<commit_message>
Added SOD523, renamed connectors library, added header to xlsx (without Footprint)
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Temp\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2E74D4-DECA-41DA-A1A0-A4D0A7E1289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBF8C45-C8EF-4DC7-88E8-962F8A493519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" firstSheet="1" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="7164" yWindow="3444" windowWidth="23040" windowHeight="12120" firstSheet="2" activeTab="8" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16046" uniqueCount="4506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16087" uniqueCount="4526">
   <si>
     <t>Part Number</t>
   </si>
@@ -13239,9 +13239,6 @@
     <t>M3x0.5, 2mm</t>
   </si>
   <si>
-    <t>SCH/Con.SchLib</t>
-  </si>
-  <si>
     <t>CON1</t>
   </si>
   <si>
@@ -13368,9 +13365,6 @@
     <t>SCH/ESP8266.SchLib</t>
   </si>
   <si>
-    <t>PCB/ESP8266.PcbLib</t>
-  </si>
-  <si>
     <t>https://www.microchip.ua/wireless/esp01.pdf</t>
   </si>
   <si>
@@ -13564,6 +13558,72 @@
   </si>
   <si>
     <t>C6807797</t>
+  </si>
+  <si>
+    <t>BAS70-02V-G3-08</t>
+  </si>
+  <si>
+    <t>SOD1608X065</t>
+  </si>
+  <si>
+    <t>Small Signal Schottky Diode</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>SOD523</t>
+  </si>
+  <si>
+    <t>70V/100mA</t>
+  </si>
+  <si>
+    <t>https://www.vishay.com/docs/85652/bas70-02v.pdf</t>
+  </si>
+  <si>
+    <t>Vishay General Semiconductor - Diodes Division</t>
+  </si>
+  <si>
+    <t>112-BAS70-02V-G3-08CT-ND</t>
+  </si>
+  <si>
+    <t>Vishay Intertech</t>
+  </si>
+  <si>
+    <t>C3313114</t>
+  </si>
+  <si>
+    <t>P-CH 20V Fast Switching MOSFETs</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2306211455_HL-3415_C7431444.pdf</t>
+  </si>
+  <si>
+    <t>C7431444</t>
+  </si>
+  <si>
+    <t>HL 2302</t>
+  </si>
+  <si>
+    <t>HL 3415</t>
+  </si>
+  <si>
+    <t>HL</t>
+  </si>
+  <si>
+    <t>Header_2x4</t>
+  </si>
+  <si>
+    <t>Header 100 mil</t>
+  </si>
+  <si>
+    <t>CON8</t>
+  </si>
+  <si>
+    <t>SCH/Connector.SchLib</t>
+  </si>
+  <si>
+    <t>PCB/ESP8622.PcbLib</t>
   </si>
 </sst>
 </file>
@@ -14261,13 +14321,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8992C59-F5E3-466D-8132-19915B114D9C}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14278,7 +14338,7 @@
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
@@ -14371,7 +14431,7 @@
         <v>2697</v>
       </c>
       <c r="H2" t="s">
-        <v>4465</v>
+        <v>4463</v>
       </c>
       <c r="I2" t="s">
         <v>2703</v>
@@ -14415,7 +14475,7 @@
         <v>2711</v>
       </c>
       <c r="H3" t="s">
-        <v>4466</v>
+        <v>4464</v>
       </c>
       <c r="I3" t="s">
         <v>2712</v>
@@ -14456,7 +14516,7 @@
         <v>2714</v>
       </c>
       <c r="H4" t="s">
-        <v>4465</v>
+        <v>4463</v>
       </c>
       <c r="I4" t="s">
         <v>2703</v>
@@ -14743,302 +14803,346 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>4457</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4457</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4458</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4462</v>
+      </c>
+      <c r="E11" t="s">
         <v>4459</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4459</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4460</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4464</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4461</v>
       </c>
       <c r="F11" t="s">
         <v>2704</v>
       </c>
       <c r="G11" t="s">
-        <v>4459</v>
+        <v>4457</v>
       </c>
       <c r="H11" t="s">
-        <v>4465</v>
+        <v>4463</v>
       </c>
       <c r="I11" t="s">
         <v>2703</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>4467</v>
+        <v>4465</v>
       </c>
       <c r="K11" t="s">
-        <v>4464</v>
+        <v>4462</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>4462</v>
+        <v>4460</v>
       </c>
       <c r="M11" t="s">
         <v>2700</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>4463</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>4466</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4466</v>
+      </c>
+      <c r="C12" t="s">
         <v>4468</v>
       </c>
-      <c r="B12" t="s">
-        <v>4468</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4470</v>
-      </c>
       <c r="D12" t="s">
+        <v>4467</v>
+      </c>
+      <c r="E12" t="s">
         <v>4469</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4471</v>
       </c>
       <c r="F12" t="s">
         <v>2704</v>
       </c>
       <c r="G12" t="s">
-        <v>4474</v>
+        <v>4472</v>
       </c>
       <c r="H12" t="s">
+        <v>4464</v>
+      </c>
+      <c r="I12" t="s">
+        <v>4473</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>4471</v>
+      </c>
+      <c r="K12" t="s">
+        <v>4467</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>4466</v>
-      </c>
-      <c r="I12" t="s">
-        <v>4475</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>4473</v>
-      </c>
-      <c r="K12" t="s">
-        <v>4469</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>4468</v>
       </c>
       <c r="M12" t="s">
         <v>2700</v>
       </c>
       <c r="N12" t="s">
-        <v>4472</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4476</v>
+        <v>4474</v>
       </c>
       <c r="B13" t="s">
-        <v>4476</v>
+        <v>4474</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>4477</v>
+        <v>4475</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>4461</v>
+        <v>4459</v>
       </c>
       <c r="F13" t="s">
         <v>2704</v>
       </c>
       <c r="G13" t="s">
-        <v>4478</v>
+        <v>4476</v>
       </c>
       <c r="H13" t="s">
-        <v>4465</v>
+        <v>4463</v>
       </c>
       <c r="I13" t="s">
         <v>2703</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>4481</v>
+        <v>4479</v>
       </c>
       <c r="K13" t="s">
+        <v>4478</v>
+      </c>
+      <c r="L13" t="s">
+        <v>4474</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
+        <v>4477</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>4480</v>
       </c>
-      <c r="L13" t="s">
-        <v>4476</v>
-      </c>
-      <c r="M13" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" t="s">
-        <v>4479</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>4482</v>
-      </c>
       <c r="P13" t="s">
-        <v>4476</v>
+        <v>4474</v>
       </c>
       <c r="Q13" t="s">
         <v>2700</v>
       </c>
       <c r="R13" t="s">
-        <v>4483</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4484</v>
+        <v>4482</v>
       </c>
       <c r="B14" t="s">
-        <v>4484</v>
+        <v>4482</v>
       </c>
       <c r="C14" t="s">
-        <v>4489</v>
+        <v>4487</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>4461</v>
+        <v>4459</v>
       </c>
       <c r="F14" t="s">
         <v>2704</v>
       </c>
       <c r="G14" t="s">
-        <v>4488</v>
+        <v>4486</v>
       </c>
       <c r="H14" t="s">
-        <v>4465</v>
+        <v>4463</v>
       </c>
       <c r="I14" t="s">
         <v>2703</v>
       </c>
       <c r="J14" t="s">
-        <v>4487</v>
+        <v>4485</v>
       </c>
       <c r="K14" t="s">
-        <v>4486</v>
+        <v>4484</v>
       </c>
       <c r="L14" t="s">
-        <v>4484</v>
+        <v>4482</v>
       </c>
       <c r="M14" t="s">
         <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>4485</v>
+        <v>4483</v>
       </c>
       <c r="O14" t="s">
-        <v>4490</v>
+        <v>4488</v>
       </c>
       <c r="P14" t="s">
-        <v>4484</v>
+        <v>4482</v>
       </c>
       <c r="Q14" t="s">
         <v>2700</v>
       </c>
       <c r="R14" t="s">
-        <v>4491</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4492</v>
+        <v>4490</v>
       </c>
       <c r="B15" t="s">
-        <v>4492</v>
+        <v>4490</v>
       </c>
       <c r="C15" t="s">
-        <v>4493</v>
+        <v>4491</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>4461</v>
+        <v>4459</v>
       </c>
       <c r="F15" t="s">
         <v>2704</v>
       </c>
       <c r="G15" t="s">
-        <v>4478</v>
+        <v>4476</v>
       </c>
       <c r="H15" t="s">
-        <v>4465</v>
+        <v>4463</v>
       </c>
       <c r="I15" t="s">
         <v>2703</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>4492</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>4493</v>
+      </c>
+      <c r="L15" t="s">
+        <v>4495</v>
+      </c>
+      <c r="M15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" t="s">
         <v>4494</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>4495</v>
-      </c>
-      <c r="L15" t="s">
-        <v>4497</v>
-      </c>
-      <c r="M15" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" t="s">
-        <v>4496</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2302</v>
       </c>
-      <c r="B16">
-        <v>2302</v>
+      <c r="B16" t="s">
+        <v>4518</v>
       </c>
       <c r="C16" t="s">
-        <v>4499</v>
+        <v>4497</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>4461</v>
+        <v>4459</v>
       </c>
       <c r="F16" t="s">
         <v>2704</v>
       </c>
       <c r="G16" t="s">
-        <v>4478</v>
+        <v>4476</v>
       </c>
       <c r="H16" t="s">
-        <v>4465</v>
+        <v>4463</v>
       </c>
       <c r="I16" t="s">
-        <v>4475</v>
+        <v>4473</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>4501</v>
+        <v>4499</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>4500</v>
+        <v>4498</v>
       </c>
       <c r="L16" t="s">
-        <v>4498</v>
+        <v>4496</v>
       </c>
       <c r="M16" t="s">
         <v>2700</v>
       </c>
       <c r="N16" t="s">
+        <v>4500</v>
+      </c>
+      <c r="O16" s="5" t="s">
         <v>4502</v>
       </c>
-      <c r="O16" s="5" t="s">
-        <v>4504</v>
-      </c>
       <c r="P16" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="Q16" t="s">
         <v>2700</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>4505</v>
+        <v>4503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4519</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4519</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4515</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4459</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2704</v>
+      </c>
+      <c r="G17" t="s">
+        <v>4486</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4463</v>
+      </c>
+      <c r="I17" t="s">
+        <v>2703</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>4516</v>
+      </c>
+      <c r="K17" t="s">
+        <v>4520</v>
+      </c>
+      <c r="L17" t="s">
+        <v>4519</v>
+      </c>
+      <c r="M17" t="s">
+        <v>2700</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>4517</v>
       </c>
     </row>
   </sheetData>
@@ -15056,7 +15160,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15151,13 +15255,13 @@
         <v>4391</v>
       </c>
       <c r="F2" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G2" t="s">
         <v>4392</v>
       </c>
       <c r="H2" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
       <c r="I2" t="s">
         <v>4389</v>
@@ -15165,210 +15269,210 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>4407</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4409</v>
+      </c>
+      <c r="C3" t="s">
         <v>4408</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4410</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4409</v>
       </c>
       <c r="D3" t="s">
         <v>4391</v>
       </c>
       <c r="F3" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G3" t="s">
         <v>4392</v>
       </c>
       <c r="H3" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
       <c r="I3" t="s">
-        <v>4408</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>4412</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4414</v>
+      </c>
+      <c r="C4" t="s">
         <v>4413</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4415</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4414</v>
       </c>
       <c r="D4" t="s">
         <v>4391</v>
       </c>
       <c r="F4" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G4" t="s">
         <v>4392</v>
       </c>
       <c r="H4" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
       <c r="I4" t="s">
-        <v>4413</v>
+        <v>4412</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4416</v>
+        <v>4415</v>
       </c>
       <c r="B5" t="s">
-        <v>4420</v>
+        <v>4419</v>
       </c>
       <c r="C5" t="s">
-        <v>4427</v>
+        <v>4426</v>
       </c>
       <c r="D5" t="s">
         <v>4391</v>
       </c>
       <c r="F5" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G5" t="s">
-        <v>4411</v>
+        <v>4410</v>
       </c>
       <c r="H5" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
       <c r="I5" t="s">
-        <v>4416</v>
+        <v>4415</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4417</v>
+        <v>4416</v>
       </c>
       <c r="B6" t="s">
-        <v>4421</v>
+        <v>4420</v>
       </c>
       <c r="C6" t="s">
-        <v>4426</v>
+        <v>4425</v>
       </c>
       <c r="D6" t="s">
         <v>4391</v>
       </c>
       <c r="F6" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G6" t="s">
-        <v>4411</v>
+        <v>4410</v>
       </c>
       <c r="H6" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
       <c r="I6" t="s">
-        <v>4417</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4418</v>
+        <v>4417</v>
       </c>
       <c r="B7" t="s">
-        <v>4422</v>
+        <v>4421</v>
       </c>
       <c r="C7" t="s">
-        <v>4425</v>
+        <v>4424</v>
       </c>
       <c r="D7" t="s">
         <v>4391</v>
       </c>
       <c r="F7" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G7" t="s">
-        <v>4412</v>
+        <v>4411</v>
       </c>
       <c r="H7" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
       <c r="I7" t="s">
-        <v>4418</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4419</v>
+        <v>4418</v>
       </c>
       <c r="B8" t="s">
+        <v>4422</v>
+      </c>
+      <c r="C8" t="s">
         <v>4423</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4424</v>
       </c>
       <c r="D8" t="s">
         <v>4391</v>
       </c>
       <c r="F8" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G8" t="s">
-        <v>4412</v>
+        <v>4411</v>
       </c>
       <c r="H8" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
       <c r="I8" t="s">
-        <v>4419</v>
+        <v>4418</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>4402</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4402</v>
+      </c>
+      <c r="C9" t="s">
         <v>4403</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4403</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4404</v>
       </c>
       <c r="D9" t="s">
         <v>4391</v>
       </c>
       <c r="F9" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G9" t="s">
+        <v>4405</v>
+      </c>
+      <c r="H9" t="s">
         <v>4406</v>
       </c>
-      <c r="H9" t="s">
-        <v>4407</v>
-      </c>
       <c r="I9" t="s">
-        <v>4403</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4402</v>
+        <v>4401</v>
       </c>
       <c r="B10" t="s">
-        <v>4402</v>
+        <v>4401</v>
       </c>
       <c r="C10" t="s">
-        <v>4405</v>
+        <v>4404</v>
       </c>
       <c r="D10" t="s">
         <v>4391</v>
       </c>
       <c r="F10" t="s">
-        <v>4397</v>
+        <v>4524</v>
       </c>
       <c r="G10" t="s">
+        <v>4405</v>
+      </c>
+      <c r="H10" t="s">
         <v>4406</v>
       </c>
-      <c r="H10" t="s">
-        <v>4407</v>
-      </c>
       <c r="I10" t="s">
-        <v>4402</v>
+        <v>4401</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -15385,66 +15489,66 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
+        <v>4524</v>
+      </c>
+      <c r="G11" t="s">
         <v>4397</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>4398</v>
       </c>
-      <c r="H11" t="s">
-        <v>4399</v>
-      </c>
       <c r="I11" t="s">
-        <v>4401</v>
+        <v>4400</v>
       </c>
       <c r="K11" t="s">
+        <v>4427</v>
+      </c>
+      <c r="L11" t="s">
         <v>4428</v>
-      </c>
-      <c r="L11" t="s">
-        <v>4429</v>
       </c>
       <c r="M11" t="s">
         <v>2700</v>
       </c>
       <c r="N11" t="s">
+        <v>4429</v>
+      </c>
+      <c r="O11" t="s">
         <v>4430</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>4431</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
+        <v>4433</v>
+      </c>
+      <c r="R11" s="9" t="s">
         <v>4432</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>4434</v>
-      </c>
-      <c r="R11" s="9" t="s">
-        <v>4433</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4444</v>
+        <v>4442</v>
       </c>
       <c r="B12" t="s">
-        <v>4444</v>
+        <v>4442</v>
       </c>
       <c r="C12" t="s">
-        <v>4445</v>
+        <v>4443</v>
       </c>
       <c r="D12" t="s">
         <v>4391</v>
       </c>
       <c r="F12" t="s">
+        <v>4444</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4445</v>
+      </c>
+      <c r="H12" t="s">
         <v>4446</v>
       </c>
-      <c r="G12" t="s">
-        <v>4447</v>
-      </c>
-      <c r="H12" t="s">
-        <v>4448</v>
-      </c>
       <c r="I12" t="s">
-        <v>4444</v>
+        <v>4442</v>
       </c>
     </row>
   </sheetData>
@@ -36118,13 +36222,13 @@
     </row>
     <row r="343" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>4449</v>
+        <v>4447</v>
       </c>
       <c r="B343" t="s">
-        <v>4449</v>
+        <v>4447</v>
       </c>
       <c r="C343" t="s">
-        <v>4450</v>
+        <v>4448</v>
       </c>
       <c r="D343" t="s">
         <v>21</v>
@@ -36133,50 +36237,50 @@
         <v>1206</v>
       </c>
       <c r="F343" t="s">
-        <v>4451</v>
+        <v>4449</v>
       </c>
       <c r="G343" t="str">
         <f>Config!$B$3</f>
         <v>SCH/R_IEC.SchLib</v>
       </c>
       <c r="H343" t="s">
-        <v>4452</v>
+        <v>4450</v>
       </c>
       <c r="I343" t="s">
         <v>469</v>
       </c>
       <c r="J343" t="s">
-        <v>4453</v>
+        <v>4451</v>
       </c>
       <c r="K343" s="4">
         <v>1.5</v>
       </c>
       <c r="L343" s="5" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
       <c r="M343" s="5" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
       <c r="N343" t="s">
+        <v>4453</v>
+      </c>
+      <c r="O343" t="s">
+        <v>26</v>
+      </c>
+      <c r="P343" t="s">
+        <v>4452</v>
+      </c>
+      <c r="Q343" s="5" t="s">
         <v>4455</v>
       </c>
-      <c r="O343" t="s">
-        <v>26</v>
-      </c>
-      <c r="P343" t="s">
-        <v>4454</v>
-      </c>
-      <c r="Q343" s="5" t="s">
-        <v>4457</v>
-      </c>
       <c r="R343" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
       <c r="S343" t="s">
         <v>2700</v>
       </c>
       <c r="T343" s="10" t="s">
-        <v>4458</v>
+        <v>4456</v>
       </c>
     </row>
   </sheetData>
@@ -42009,13 +42113,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6596218-16F3-44AE-9E9B-CCA683897864}">
-  <dimension ref="A1:T494"/>
+  <dimension ref="A1:T495"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C470" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
+      <selection pane="bottomRight" activeCell="A496" sqref="A496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68222,6 +68326,68 @@
         <v>4372</v>
       </c>
     </row>
+    <row r="495" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A495" t="s">
+        <v>4504</v>
+      </c>
+      <c r="B495" t="s">
+        <v>4504</v>
+      </c>
+      <c r="C495" t="s">
+        <v>4506</v>
+      </c>
+      <c r="D495" t="s">
+        <v>4507</v>
+      </c>
+      <c r="E495" t="s">
+        <v>4508</v>
+      </c>
+      <c r="F495" t="s">
+        <v>4509</v>
+      </c>
+      <c r="G495" t="s">
+        <v>2725</v>
+      </c>
+      <c r="H495" t="s">
+        <v>4311</v>
+      </c>
+      <c r="I495" t="s">
+        <v>2726</v>
+      </c>
+      <c r="J495" t="s">
+        <v>4505</v>
+      </c>
+      <c r="K495" t="s">
+        <v>2988</v>
+      </c>
+      <c r="L495" t="s">
+        <v>4510</v>
+      </c>
+      <c r="M495" t="s">
+        <v>4511</v>
+      </c>
+      <c r="N495" t="s">
+        <v>4504</v>
+      </c>
+      <c r="O495" t="s">
+        <v>26</v>
+      </c>
+      <c r="P495" t="s">
+        <v>4512</v>
+      </c>
+      <c r="Q495" t="s">
+        <v>4513</v>
+      </c>
+      <c r="R495" t="s">
+        <v>4504</v>
+      </c>
+      <c r="S495" t="s">
+        <v>2700</v>
+      </c>
+      <c r="T495" t="s">
+        <v>4514</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R489" r:id="rId1" display="https://www.lcsc.com/product-detail/Schottky-Barrier-Diodes-SBD_Slkor-SLKORMICRO-Elec-SS26_C513477.html" xr:uid="{091CD993-3645-4E44-9CF4-879C490DFAC3}"/>
@@ -68233,13 +68399,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05348336-C131-49E6-98A6-4A6B8B6DDA7F}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68304,6 +68470,26 @@
       </c>
       <c r="T1" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4521</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4521</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4522</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4524</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4523</v>
       </c>
     </row>
   </sheetData>
@@ -68395,11 +68581,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE0A8F6A-F5E5-42B9-9631-24C8A730FB17}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68468,46 +68654,46 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4434</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4434</v>
+      </c>
+      <c r="C2" t="s">
         <v>4435</v>
       </c>
-      <c r="B2" t="s">
-        <v>4435</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4436</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4437</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>4438</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>4434</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4525</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4434</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>4439</v>
       </c>
-      <c r="H2" t="s">
-        <v>4435</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4440</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4435</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>4441</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>4443</v>
-      </c>
       <c r="N2" s="5" t="s">
-        <v>4435</v>
+        <v>4434</v>
       </c>
       <c r="O2" t="s">
         <v>2700</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected Schematic Symbol of TPS4056, added AS3202 MOSFET
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Temp\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F70C479-F33A-4EC9-A91C-FFD8737FBDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1495C225-204F-4E2B-87B5-6A0432B8245B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16442" uniqueCount="4682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16460" uniqueCount="4688">
   <si>
     <t>Part Number</t>
   </si>
@@ -14092,6 +14092,24 @@
   </si>
   <si>
     <t>SOT2395P280X125-6</t>
+  </si>
+  <si>
+    <t>AS2302</t>
+  </si>
+  <si>
+    <t>N-Channel 20V(D-S) MOSFET</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1809211431_AnBon-AS2302_C232266.pdf</t>
+  </si>
+  <si>
+    <t>4530-AS2302CT-ND</t>
+  </si>
+  <si>
+    <t>AnBon</t>
+  </si>
+  <si>
+    <t>C232266</t>
   </si>
 </sst>
 </file>
@@ -14789,13 +14807,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8992C59-F5E3-466D-8132-19915B114D9C}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15755,6 +15773,62 @@
       </c>
       <c r="N20" s="8" t="s">
         <v>4676</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4682</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4682</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4683</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>4453</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2699</v>
+      </c>
+      <c r="G21" t="s">
+        <v>4470</v>
+      </c>
+      <c r="H21" t="s">
+        <v>4457</v>
+      </c>
+      <c r="I21" t="s">
+        <v>2698</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>4684</v>
+      </c>
+      <c r="K21" t="s">
+        <v>4472</v>
+      </c>
+      <c r="L21" t="s">
+        <v>4682</v>
+      </c>
+      <c r="M21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" t="s">
+        <v>4685</v>
+      </c>
+      <c r="O21" t="s">
+        <v>4686</v>
+      </c>
+      <c r="P21" t="s">
+        <v>4682</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>2695</v>
+      </c>
+      <c r="R21" t="s">
+        <v>4687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LCSC HelpURL corrected, PEM renamed
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E998BB-C6C8-4F4F-B78E-2C3EA678F75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6A5C5A-CECD-47D0-BB40-69868DF4DF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="17325" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16495" uniqueCount="4707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16495" uniqueCount="4706">
   <si>
     <t>Part Number</t>
   </si>
@@ -13179,15 +13179,9 @@
     <t>D_Zener</t>
   </si>
   <si>
-    <t>SMTSO3020CTJ</t>
-  </si>
-  <si>
     <t>Solder Nut M3x0.5, 2mm</t>
   </si>
   <si>
-    <t>M3x0.5, 2mm</t>
-  </si>
-  <si>
     <t>CON1</t>
   </si>
   <si>
@@ -13956,57 +13950,6 @@
     <t>LCSC</t>
   </si>
   <si>
-    <t>https://datasheet.LCSC/lcsc/2202131930_MSKSEMI-SS24-MS_C2836395.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/1912111437_PUOLOP-DW01A_C351410.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2308080947_MSKSEMI-TP4056-MS_C7473158.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2401050929_JSMSEMI-8205S_C2762930.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/1810231212_Worldsemi-WS2813E_C160214.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2012110135_Worldsemi-WS2813B-V5_C965558.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2310251544_Worldsemi-WS2813B-MINI-V1_C2832664.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2206131216_Worldsemi-WS2812B-V5-W_C2874885.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2111171930_Worldsemi-WS2812E-V5_C2920042.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2005251033_Worldsemi-WS2812B-Mini_C527089.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/1811061532_UTC-Unisonic-Tech-UHE4913G-AE3-R_C86815.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2212101330_XINLUDA-XL555_C521186.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2009171007_HUASHUO-HSS2302B_C518782.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2306211455_HL-3415_C7431444.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2203221830_Zetta-ZD8028IB5TR_C2928932.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/2307141446_JSMSEMI-2N7002_C916396.pdf</t>
-  </si>
-  <si>
-    <t>https://datasheet.LCSC/lcsc/1809211431_AnBon-AS2302_C232266.pdf</t>
-  </si>
-  <si>
     <t>470NH/2520</t>
   </si>
   <si>
@@ -14167,6 +14110,60 @@
   </si>
   <si>
     <t>MMBT4403L</t>
+  </si>
+  <si>
+    <t>PEM M3, 2mm</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2202131930_MSKSEMI-SS24-MS_C2836395.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1912111437_PUOLOP-DW01A_C351410.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2308080947_MSKSEMI-TP4056-MS_C7473158.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2401050929_JSMSEMI-8205S_C2762930.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1810231212_Worldsemi-WS2813E_C160214.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2012110135_Worldsemi-WS2813B-V5_C965558.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2310251544_Worldsemi-WS2813B-MINI-V1_C2832664.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2206131216_Worldsemi-WS2812B-V5-W_C2874885.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2111171930_Worldsemi-WS2812E-V5_C2920042.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2005251033_Worldsemi-WS2812B-Mini_C527089.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1811061532_UTC-Unisonic-Tech-UHE4913G-AE3-R_C86815.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2212101330_XINLUDA-XL555_C521186.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2009171007_HUASHUO-HSS2302B_C518782.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2306211455_HL-3415_C7431444.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2203221830_Zetta-ZD8028IB5TR_C2928932.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2307141446_JSMSEMI-2N7002_C916396.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1809211431_AnBon-AS2302_C232266.pdf</t>
   </si>
 </sst>
 </file>
@@ -14871,7 +14868,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -14975,13 +14972,13 @@
         <v>2692</v>
       </c>
       <c r="H2" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I2" t="s">
         <v>2696</v>
       </c>
       <c r="J2" t="s">
-        <v>4637</v>
+        <v>4690</v>
       </c>
       <c r="K2" t="s">
         <v>2694</v>
@@ -14990,7 +14987,7 @@
         <v>2692</v>
       </c>
       <c r="M2" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N2" t="s">
         <v>2695</v>
@@ -15019,13 +15016,13 @@
         <v>2703</v>
       </c>
       <c r="H3" t="s">
-        <v>4447</v>
+        <v>4445</v>
       </c>
       <c r="I3" t="s">
         <v>2704</v>
       </c>
       <c r="J3" t="s">
-        <v>4638</v>
+        <v>4691</v>
       </c>
       <c r="K3" t="s">
         <v>2701</v>
@@ -15034,7 +15031,7 @@
         <v>2699</v>
       </c>
       <c r="M3" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N3" t="s">
         <v>2705</v>
@@ -15060,13 +15057,13 @@
         <v>2706</v>
       </c>
       <c r="H4" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I4" t="s">
-        <v>4629</v>
+        <v>4627</v>
       </c>
       <c r="J4" t="s">
-        <v>4639</v>
+        <v>4692</v>
       </c>
       <c r="K4" t="s">
         <v>2709</v>
@@ -15075,7 +15072,7 @@
         <v>2707</v>
       </c>
       <c r="M4" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N4" t="s">
         <v>2710</v>
@@ -15110,7 +15107,7 @@
         <v>4282</v>
       </c>
       <c r="J5" t="s">
-        <v>4640</v>
+        <v>4693</v>
       </c>
       <c r="K5" t="s">
         <v>3907</v>
@@ -15119,7 +15116,7 @@
         <v>3584</v>
       </c>
       <c r="M5" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N5" t="s">
         <v>4286</v>
@@ -15154,7 +15151,7 @@
         <v>4282</v>
       </c>
       <c r="J6" t="s">
-        <v>4641</v>
+        <v>4694</v>
       </c>
       <c r="K6" t="s">
         <v>3907</v>
@@ -15163,7 +15160,7 @@
         <v>3911</v>
       </c>
       <c r="M6" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N6" t="s">
         <v>4288</v>
@@ -15198,7 +15195,7 @@
         <v>4285</v>
       </c>
       <c r="J7" t="s">
-        <v>4642</v>
+        <v>4695</v>
       </c>
       <c r="K7" t="s">
         <v>3907</v>
@@ -15207,7 +15204,7 @@
         <v>4287</v>
       </c>
       <c r="M7" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N7" t="s">
         <v>4289</v>
@@ -15242,7 +15239,7 @@
         <v>4283</v>
       </c>
       <c r="J8" t="s">
-        <v>4643</v>
+        <v>4696</v>
       </c>
       <c r="K8" t="s">
         <v>3907</v>
@@ -15251,7 +15248,7 @@
         <v>4290</v>
       </c>
       <c r="M8" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N8" t="s">
         <v>4291</v>
@@ -15286,7 +15283,7 @@
         <v>4283</v>
       </c>
       <c r="J9" t="s">
-        <v>4644</v>
+        <v>4697</v>
       </c>
       <c r="K9" t="s">
         <v>3907</v>
@@ -15295,7 +15292,7 @@
         <v>3910</v>
       </c>
       <c r="M9" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N9" t="s">
         <v>4292</v>
@@ -15330,7 +15327,7 @@
         <v>4284</v>
       </c>
       <c r="J10" t="s">
-        <v>4645</v>
+        <v>4698</v>
       </c>
       <c r="K10" t="s">
         <v>3907</v>
@@ -15339,7 +15336,7 @@
         <v>4294</v>
       </c>
       <c r="M10" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N10" t="s">
         <v>4293</v>
@@ -15347,246 +15344,246 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
+        <v>4438</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4438</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4439</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4443</v>
+      </c>
+      <c r="E11" t="s">
         <v>4440</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4440</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4441</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4445</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4442</v>
       </c>
       <c r="F11" t="s">
         <v>2697</v>
       </c>
       <c r="G11" t="s">
-        <v>4440</v>
+        <v>4438</v>
       </c>
       <c r="H11" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I11" t="s">
         <v>2696</v>
       </c>
       <c r="J11" t="s">
-        <v>4646</v>
+        <v>4699</v>
       </c>
       <c r="K11" t="s">
-        <v>4445</v>
+        <v>4443</v>
       </c>
       <c r="L11" t="s">
-        <v>4443</v>
+        <v>4441</v>
       </c>
       <c r="M11" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>4444</v>
+        <v>4442</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
+        <v>4446</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4446</v>
+      </c>
+      <c r="C12" t="s">
         <v>4448</v>
       </c>
-      <c r="B12" t="s">
-        <v>4448</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4450</v>
-      </c>
       <c r="D12" t="s">
+        <v>4447</v>
+      </c>
+      <c r="E12" t="s">
         <v>4449</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4451</v>
       </c>
       <c r="F12" t="s">
         <v>2697</v>
       </c>
       <c r="G12" t="s">
-        <v>4453</v>
+        <v>4451</v>
       </c>
       <c r="H12" t="s">
+        <v>4445</v>
+      </c>
+      <c r="I12" t="s">
+        <v>4452</v>
+      </c>
+      <c r="J12" t="s">
+        <v>4700</v>
+      </c>
+      <c r="K12" t="s">
         <v>4447</v>
       </c>
-      <c r="I12" t="s">
-        <v>4454</v>
-      </c>
-      <c r="J12" t="s">
-        <v>4647</v>
-      </c>
-      <c r="K12" t="s">
-        <v>4449</v>
-      </c>
       <c r="L12" t="s">
-        <v>4448</v>
+        <v>4446</v>
       </c>
       <c r="M12" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N12" t="s">
-        <v>4452</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
       <c r="B13" t="s">
-        <v>4455</v>
+        <v>4453</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>4456</v>
+        <v>4454</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="F13" t="s">
         <v>2697</v>
       </c>
       <c r="G13" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
       <c r="H13" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I13" t="s">
         <v>2696</v>
       </c>
       <c r="J13" t="s">
+        <v>4458</v>
+      </c>
+      <c r="K13" t="s">
+        <v>4457</v>
+      </c>
+      <c r="L13" t="s">
+        <v>4453</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
+        <v>4456</v>
+      </c>
+      <c r="O13" t="s">
+        <v>4459</v>
+      </c>
+      <c r="P13" t="s">
+        <v>4453</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>4633</v>
+      </c>
+      <c r="R13" t="s">
         <v>4460</v>
-      </c>
-      <c r="K13" t="s">
-        <v>4459</v>
-      </c>
-      <c r="L13" t="s">
-        <v>4455</v>
-      </c>
-      <c r="M13" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" t="s">
-        <v>4458</v>
-      </c>
-      <c r="O13" t="s">
-        <v>4461</v>
-      </c>
-      <c r="P13" t="s">
-        <v>4455</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>4635</v>
-      </c>
-      <c r="R13" t="s">
-        <v>4462</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>4463</v>
+        <v>4461</v>
       </c>
       <c r="B14" t="s">
-        <v>4463</v>
+        <v>4461</v>
       </c>
       <c r="C14" t="s">
-        <v>4468</v>
+        <v>4466</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="F14" t="s">
         <v>2697</v>
       </c>
       <c r="G14" t="s">
-        <v>4467</v>
+        <v>4465</v>
       </c>
       <c r="H14" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I14" t="s">
         <v>2696</v>
       </c>
       <c r="J14" t="s">
-        <v>4466</v>
+        <v>4464</v>
       </c>
       <c r="K14" t="s">
-        <v>4465</v>
+        <v>4463</v>
       </c>
       <c r="L14" t="s">
-        <v>4463</v>
+        <v>4461</v>
       </c>
       <c r="M14" t="s">
         <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>4464</v>
+        <v>4462</v>
       </c>
       <c r="O14" t="s">
-        <v>4469</v>
+        <v>4467</v>
       </c>
       <c r="P14" t="s">
-        <v>4463</v>
+        <v>4461</v>
       </c>
       <c r="Q14" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="R14" t="s">
-        <v>4470</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>4471</v>
+        <v>4469</v>
       </c>
       <c r="B15" t="s">
-        <v>4471</v>
+        <v>4469</v>
       </c>
       <c r="C15" t="s">
-        <v>4472</v>
+        <v>4470</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="F15" t="s">
         <v>2697</v>
       </c>
       <c r="G15" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
       <c r="H15" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I15" t="s">
         <v>2696</v>
       </c>
       <c r="J15" t="s">
+        <v>4471</v>
+      </c>
+      <c r="K15" t="s">
+        <v>4472</v>
+      </c>
+      <c r="L15" t="s">
+        <v>4474</v>
+      </c>
+      <c r="M15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N15" t="s">
         <v>4473</v>
-      </c>
-      <c r="K15" t="s">
-        <v>4474</v>
-      </c>
-      <c r="L15" t="s">
-        <v>4476</v>
-      </c>
-      <c r="M15" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" t="s">
-        <v>4475</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -15594,231 +15591,231 @@
         <v>2302</v>
       </c>
       <c r="B16" t="s">
-        <v>4497</v>
+        <v>4495</v>
       </c>
       <c r="C16" t="s">
-        <v>4478</v>
+        <v>4476</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="F16" t="s">
         <v>2697</v>
       </c>
       <c r="G16" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
       <c r="H16" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I16" t="s">
-        <v>4454</v>
+        <v>4452</v>
       </c>
       <c r="J16" t="s">
-        <v>4648</v>
+        <v>4701</v>
       </c>
       <c r="K16" t="s">
+        <v>4477</v>
+      </c>
+      <c r="L16" t="s">
+        <v>4475</v>
+      </c>
+      <c r="M16" t="s">
+        <v>4633</v>
+      </c>
+      <c r="N16" t="s">
+        <v>4478</v>
+      </c>
+      <c r="O16" t="s">
+        <v>4480</v>
+      </c>
+      <c r="P16" t="s">
         <v>4479</v>
       </c>
-      <c r="L16" t="s">
-        <v>4477</v>
-      </c>
-      <c r="M16" t="s">
-        <v>4635</v>
-      </c>
-      <c r="N16" t="s">
-        <v>4480</v>
-      </c>
-      <c r="O16" t="s">
-        <v>4482</v>
-      </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
+        <v>4633</v>
+      </c>
+      <c r="R16" t="s">
         <v>4481</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>4635</v>
-      </c>
-      <c r="R16" t="s">
-        <v>4483</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>4498</v>
+        <v>4496</v>
       </c>
       <c r="B17" t="s">
-        <v>4498</v>
+        <v>4496</v>
       </c>
       <c r="C17" t="s">
-        <v>4495</v>
+        <v>4493</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="F17" t="s">
         <v>2697</v>
       </c>
       <c r="G17" t="s">
-        <v>4467</v>
+        <v>4465</v>
       </c>
       <c r="H17" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I17" t="s">
         <v>2696</v>
       </c>
       <c r="J17" t="s">
-        <v>4649</v>
+        <v>4702</v>
       </c>
       <c r="K17" t="s">
-        <v>4499</v>
+        <v>4497</v>
       </c>
       <c r="L17" t="s">
-        <v>4498</v>
+        <v>4496</v>
       </c>
       <c r="M17" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>4496</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>4593</v>
+        <v>4591</v>
       </c>
       <c r="B18" t="s">
-        <v>4593</v>
+        <v>4591</v>
       </c>
       <c r="C18" t="s">
-        <v>4592</v>
+        <v>4590</v>
       </c>
       <c r="D18" t="s">
-        <v>4590</v>
+        <v>4588</v>
       </c>
       <c r="E18" t="s">
-        <v>4596</v>
+        <v>4594</v>
       </c>
       <c r="F18" t="s">
         <v>2697</v>
       </c>
       <c r="G18" t="s">
+        <v>4591</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4444</v>
+      </c>
+      <c r="I18" t="s">
+        <v>4595</v>
+      </c>
+      <c r="J18" t="s">
         <v>4593</v>
       </c>
-      <c r="H18" t="s">
-        <v>4446</v>
-      </c>
-      <c r="I18" t="s">
-        <v>4597</v>
-      </c>
-      <c r="J18" t="s">
-        <v>4595</v>
-      </c>
       <c r="K18" t="s">
-        <v>4590</v>
+        <v>4588</v>
       </c>
       <c r="L18" t="s">
-        <v>4593</v>
+        <v>4591</v>
       </c>
       <c r="M18" t="s">
         <v>26</v>
       </c>
       <c r="N18" t="s">
-        <v>4594</v>
+        <v>4592</v>
       </c>
       <c r="O18" t="s">
-        <v>4590</v>
+        <v>4588</v>
       </c>
       <c r="P18" t="s">
-        <v>4593</v>
+        <v>4591</v>
       </c>
       <c r="Q18" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>4591</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="8" t="s">
-        <v>4602</v>
+        <v>4600</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>4602</v>
+        <v>4600</v>
       </c>
       <c r="C19" t="s">
-        <v>4603</v>
+        <v>4601</v>
       </c>
       <c r="D19" t="s">
-        <v>4600</v>
+        <v>4598</v>
       </c>
       <c r="E19" t="s">
-        <v>4628</v>
+        <v>4626</v>
       </c>
       <c r="F19" t="s">
         <v>2697</v>
       </c>
       <c r="G19" t="s">
-        <v>4602</v>
+        <v>4600</v>
       </c>
       <c r="H19" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I19" t="s">
-        <v>4601</v>
+        <v>4599</v>
       </c>
       <c r="J19" t="s">
-        <v>4650</v>
+        <v>4703</v>
       </c>
       <c r="K19" t="s">
-        <v>4600</v>
+        <v>4598</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>4598</v>
+        <v>4596</v>
       </c>
       <c r="M19" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>4599</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="8" t="s">
-        <v>4626</v>
+        <v>4624</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>4626</v>
+        <v>4624</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>4627</v>
+        <v>4625</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="F20" t="s">
         <v>2697</v>
       </c>
       <c r="G20" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
       <c r="H20" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I20" t="s">
         <v>2696</v>
       </c>
       <c r="J20" t="s">
-        <v>4651</v>
+        <v>4704</v>
       </c>
       <c r="K20" t="s">
         <v>2709</v>
@@ -15827,110 +15824,110 @@
         <v>2709</v>
       </c>
       <c r="M20" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>4625</v>
+        <v>4623</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>4630</v>
+        <v>4628</v>
       </c>
       <c r="B21" t="s">
-        <v>4630</v>
+        <v>4628</v>
       </c>
       <c r="C21" t="s">
-        <v>4631</v>
+        <v>4629</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="F21" t="s">
         <v>2697</v>
       </c>
       <c r="G21" t="s">
-        <v>4457</v>
+        <v>4455</v>
       </c>
       <c r="H21" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I21" t="s">
         <v>2696</v>
       </c>
       <c r="J21" t="s">
-        <v>4652</v>
+        <v>4705</v>
       </c>
       <c r="K21" t="s">
-        <v>4459</v>
+        <v>4457</v>
       </c>
       <c r="L21" t="s">
+        <v>4628</v>
+      </c>
+      <c r="M21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" t="s">
         <v>4630</v>
       </c>
-      <c r="M21" t="s">
-        <v>26</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
+        <v>4631</v>
+      </c>
+      <c r="P21" t="s">
+        <v>4628</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>4633</v>
+      </c>
+      <c r="R21" t="s">
         <v>4632</v>
-      </c>
-      <c r="O21" t="s">
-        <v>4633</v>
-      </c>
-      <c r="P21" t="s">
-        <v>4630</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>4635</v>
-      </c>
-      <c r="R21" t="s">
-        <v>4634</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
-        <v>4706</v>
+        <v>4687</v>
       </c>
       <c r="B22" t="s">
-        <v>4706</v>
+        <v>4687</v>
       </c>
       <c r="C22" t="s">
-        <v>4701</v>
+        <v>4682</v>
       </c>
       <c r="D22" t="s">
-        <v>4705</v>
+        <v>4686</v>
       </c>
       <c r="E22" t="s">
-        <v>4442</v>
+        <v>4440</v>
       </c>
       <c r="F22" t="s">
         <v>2697</v>
       </c>
       <c r="G22" t="s">
-        <v>4699</v>
+        <v>4680</v>
       </c>
       <c r="H22" t="s">
-        <v>4446</v>
+        <v>4444</v>
       </c>
       <c r="I22" t="s">
         <v>2696</v>
       </c>
       <c r="J22" t="s">
-        <v>4702</v>
+        <v>4683</v>
       </c>
       <c r="K22" t="s">
-        <v>4703</v>
+        <v>4684</v>
       </c>
       <c r="L22" t="s">
-        <v>4700</v>
+        <v>4681</v>
       </c>
       <c r="M22" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>4704</v>
+        <v>4685</v>
       </c>
     </row>
   </sheetData>
@@ -15947,8 +15944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CA65D6-1BE4-4CF1-A255-E1F9C8CC291A}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -16043,13 +16040,13 @@
         <v>4374</v>
       </c>
       <c r="F2" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G2" t="s">
         <v>4375</v>
       </c>
       <c r="H2" t="s">
-        <v>4382</v>
+        <v>4380</v>
       </c>
       <c r="I2" t="s">
         <v>4372</v>
@@ -16057,286 +16054,286 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
+        <v>4388</v>
+      </c>
+      <c r="B3" t="s">
         <v>4390</v>
       </c>
-      <c r="B3" t="s">
-        <v>4392</v>
-      </c>
       <c r="C3" t="s">
-        <v>4391</v>
+        <v>4389</v>
       </c>
       <c r="D3" t="s">
         <v>4374</v>
       </c>
       <c r="F3" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G3" t="s">
         <v>4375</v>
       </c>
       <c r="H3" t="s">
-        <v>4382</v>
+        <v>4380</v>
       </c>
       <c r="I3" t="s">
-        <v>4390</v>
+        <v>4388</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
+        <v>4393</v>
+      </c>
+      <c r="B4" t="s">
         <v>4395</v>
       </c>
-      <c r="B4" t="s">
-        <v>4397</v>
-      </c>
       <c r="C4" t="s">
-        <v>4396</v>
+        <v>4394</v>
       </c>
       <c r="D4" t="s">
         <v>4374</v>
       </c>
       <c r="F4" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G4" t="s">
         <v>4375</v>
       </c>
       <c r="H4" t="s">
-        <v>4382</v>
+        <v>4380</v>
       </c>
       <c r="I4" t="s">
-        <v>4395</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>4398</v>
+        <v>4396</v>
       </c>
       <c r="B5" t="s">
-        <v>4402</v>
+        <v>4400</v>
       </c>
       <c r="C5" t="s">
-        <v>4409</v>
+        <v>4407</v>
       </c>
       <c r="D5" t="s">
         <v>4374</v>
       </c>
       <c r="F5" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G5" t="s">
-        <v>4393</v>
+        <v>4391</v>
       </c>
       <c r="H5" t="s">
-        <v>4382</v>
+        <v>4380</v>
       </c>
       <c r="I5" t="s">
-        <v>4398</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>4399</v>
+        <v>4397</v>
       </c>
       <c r="B6" t="s">
-        <v>4403</v>
+        <v>4401</v>
       </c>
       <c r="C6" t="s">
-        <v>4408</v>
+        <v>4406</v>
       </c>
       <c r="D6" t="s">
         <v>4374</v>
       </c>
       <c r="F6" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G6" t="s">
-        <v>4393</v>
+        <v>4391</v>
       </c>
       <c r="H6" t="s">
-        <v>4382</v>
+        <v>4380</v>
       </c>
       <c r="I6" t="s">
-        <v>4399</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>4400</v>
+        <v>4398</v>
       </c>
       <c r="B7" t="s">
-        <v>4404</v>
+        <v>4402</v>
       </c>
       <c r="C7" t="s">
-        <v>4407</v>
+        <v>4405</v>
       </c>
       <c r="D7" t="s">
         <v>4374</v>
       </c>
       <c r="F7" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G7" t="s">
-        <v>4394</v>
+        <v>4392</v>
       </c>
       <c r="H7" t="s">
-        <v>4382</v>
+        <v>4380</v>
       </c>
       <c r="I7" t="s">
-        <v>4400</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>4401</v>
+        <v>4399</v>
       </c>
       <c r="B8" t="s">
-        <v>4405</v>
+        <v>4403</v>
       </c>
       <c r="C8" t="s">
-        <v>4406</v>
+        <v>4404</v>
       </c>
       <c r="D8" t="s">
         <v>4374</v>
       </c>
       <c r="F8" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G8" t="s">
-        <v>4394</v>
+        <v>4392</v>
       </c>
       <c r="H8" t="s">
-        <v>4382</v>
+        <v>4380</v>
       </c>
       <c r="I8" t="s">
-        <v>4401</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>4385</v>
+        <v>4383</v>
       </c>
       <c r="B9" t="s">
-        <v>4385</v>
+        <v>4383</v>
       </c>
       <c r="C9" t="s">
-        <v>4386</v>
+        <v>4384</v>
       </c>
       <c r="D9" t="s">
         <v>4374</v>
       </c>
       <c r="F9" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G9" t="s">
-        <v>4388</v>
+        <v>4386</v>
       </c>
       <c r="H9" t="s">
-        <v>4389</v>
+        <v>4387</v>
       </c>
       <c r="I9" t="s">
-        <v>4385</v>
+        <v>4383</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>4384</v>
+        <v>4382</v>
       </c>
       <c r="B10" t="s">
-        <v>4384</v>
+        <v>4382</v>
       </c>
       <c r="C10" t="s">
-        <v>4387</v>
+        <v>4385</v>
       </c>
       <c r="D10" t="s">
         <v>4374</v>
       </c>
       <c r="F10" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G10" t="s">
-        <v>4388</v>
+        <v>4386</v>
       </c>
       <c r="H10" t="s">
-        <v>4389</v>
+        <v>4387</v>
       </c>
       <c r="I10" t="s">
-        <v>4384</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
+        <v>4688</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4688</v>
+      </c>
+      <c r="C11" t="s">
         <v>4377</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4379</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4378</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="G11" t="s">
-        <v>4380</v>
+        <v>4378</v>
       </c>
       <c r="H11" t="s">
+        <v>4379</v>
+      </c>
+      <c r="I11" t="s">
         <v>4381</v>
       </c>
-      <c r="I11" t="s">
-        <v>4383</v>
-      </c>
       <c r="K11" t="s">
+        <v>4408</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4409</v>
+      </c>
+      <c r="M11" t="s">
+        <v>4633</v>
+      </c>
+      <c r="N11" t="s">
         <v>4410</v>
       </c>
-      <c r="L11" t="s">
+      <c r="O11" t="s">
         <v>4411</v>
       </c>
-      <c r="M11" t="s">
-        <v>4635</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>4412</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
+        <v>4414</v>
+      </c>
+      <c r="R11" s="7" t="s">
         <v>4413</v>
-      </c>
-      <c r="P11" t="s">
-        <v>4414</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>4416</v>
-      </c>
-      <c r="R11" s="7" t="s">
-        <v>4415</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>4425</v>
+        <v>4423</v>
       </c>
       <c r="B12" t="s">
-        <v>4425</v>
+        <v>4423</v>
       </c>
       <c r="C12" t="s">
-        <v>4426</v>
+        <v>4424</v>
       </c>
       <c r="D12" t="s">
         <v>4374</v>
       </c>
       <c r="F12" t="s">
+        <v>4425</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4426</v>
+      </c>
+      <c r="H12" t="s">
         <v>4427</v>
       </c>
-      <c r="G12" t="s">
-        <v>4428</v>
-      </c>
-      <c r="H12" t="s">
-        <v>4429</v>
-      </c>
       <c r="I12" t="s">
-        <v>4425</v>
+        <v>4423</v>
       </c>
     </row>
   </sheetData>
@@ -16386,7 +16383,7 @@
         <v>452</v>
       </c>
       <c r="B5" t="s">
-        <v>4612</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -16394,7 +16391,7 @@
         <v>459</v>
       </c>
       <c r="B6" t="s">
-        <v>4522</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -16428,12 +16425,12 @@
         <v>455</v>
       </c>
       <c r="B120" t="s">
-        <v>4529</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="B121" t="s">
-        <v>4612</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -16441,17 +16438,17 @@
         <v>459</v>
       </c>
       <c r="B130" t="s">
-        <v>4522</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="B131" t="s">
-        <v>4523</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="B132" t="s">
-        <v>4524</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -37002,7 +36999,7 @@
         <v>4366</v>
       </c>
       <c r="S342" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T342" t="s">
         <v>4368</v>
@@ -37010,13 +37007,13 @@
     </row>
     <row r="343" spans="1:20">
       <c r="A343" t="s">
-        <v>4430</v>
+        <v>4428</v>
       </c>
       <c r="B343" t="s">
-        <v>4430</v>
+        <v>4428</v>
       </c>
       <c r="C343" t="s">
-        <v>4431</v>
+        <v>4429</v>
       </c>
       <c r="D343" t="s">
         <v>21</v>
@@ -37025,61 +37022,61 @@
         <v>1206</v>
       </c>
       <c r="F343" t="s">
-        <v>4432</v>
+        <v>4430</v>
       </c>
       <c r="G343" t="str">
         <f>Config!$B$3</f>
         <v>SCH/R_IEC.SchLib</v>
       </c>
       <c r="H343" t="s">
-        <v>4433</v>
+        <v>4431</v>
       </c>
       <c r="I343" t="s">
         <v>464</v>
       </c>
       <c r="J343" t="s">
-        <v>4434</v>
+        <v>4432</v>
       </c>
       <c r="K343" s="4">
         <v>1.5</v>
       </c>
       <c r="L343" t="s">
+        <v>4435</v>
+      </c>
+      <c r="M343" t="s">
+        <v>4436</v>
+      </c>
+      <c r="N343" t="s">
+        <v>4434</v>
+      </c>
+      <c r="O343" t="s">
+        <v>26</v>
+      </c>
+      <c r="P343" t="s">
+        <v>4433</v>
+      </c>
+      <c r="Q343" t="s">
+        <v>4436</v>
+      </c>
+      <c r="R343" t="s">
+        <v>4434</v>
+      </c>
+      <c r="S343" t="s">
+        <v>4633</v>
+      </c>
+      <c r="T343" s="8" t="s">
         <v>4437</v>
-      </c>
-      <c r="M343" t="s">
-        <v>4438</v>
-      </c>
-      <c r="N343" t="s">
-        <v>4436</v>
-      </c>
-      <c r="O343" t="s">
-        <v>26</v>
-      </c>
-      <c r="P343" t="s">
-        <v>4435</v>
-      </c>
-      <c r="Q343" t="s">
-        <v>4438</v>
-      </c>
-      <c r="R343" t="s">
-        <v>4436</v>
-      </c>
-      <c r="S343" t="s">
-        <v>4635</v>
-      </c>
-      <c r="T343" s="8" t="s">
-        <v>4439</v>
       </c>
     </row>
     <row r="344" spans="1:20" ht="15.75">
       <c r="A344" s="1" t="s">
-        <v>4613</v>
+        <v>4611</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>4613</v>
+        <v>4611</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>4614</v>
+        <v>4612</v>
       </c>
       <c r="D344" s="1" t="s">
         <v>21</v>
@@ -37088,7 +37085,7 @@
         <v>22</v>
       </c>
       <c r="F344" s="1" t="s">
-        <v>4615</v>
+        <v>4613</v>
       </c>
       <c r="G344" t="str">
         <f>Config!$B$3</f>
@@ -37113,13 +37110,13 @@
         <v>482</v>
       </c>
       <c r="N344" s="1" t="s">
-        <v>4617</v>
+        <v>4615</v>
       </c>
       <c r="O344" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P344" s="1" t="s">
-        <v>4616</v>
+        <v>4614</v>
       </c>
       <c r="Q344" s="1"/>
       <c r="R344" s="1"/>
@@ -37128,13 +37125,13 @@
     </row>
     <row r="345" spans="1:20" ht="15.75">
       <c r="A345" s="1" t="s">
-        <v>4623</v>
+        <v>4621</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>4623</v>
+        <v>4621</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>4618</v>
+        <v>4616</v>
       </c>
       <c r="D345" s="1" t="s">
         <v>21</v>
@@ -37143,7 +37140,7 @@
         <v>22</v>
       </c>
       <c r="F345" s="1" t="s">
-        <v>4624</v>
+        <v>4622</v>
       </c>
       <c r="G345" t="str">
         <f>Config!$B$3</f>
@@ -37162,19 +37159,19 @@
         <v>499000</v>
       </c>
       <c r="L345" s="3" t="s">
-        <v>4622</v>
+        <v>4620</v>
       </c>
       <c r="M345" s="1" t="s">
-        <v>4621</v>
+        <v>4619</v>
       </c>
       <c r="N345" s="1" t="s">
-        <v>4620</v>
+        <v>4618</v>
       </c>
       <c r="O345" s="1" t="s">
         <v>26</v>
       </c>
       <c r="P345" s="1" t="s">
-        <v>4619</v>
+        <v>4617</v>
       </c>
       <c r="Q345" s="1"/>
       <c r="R345" s="1"/>
@@ -42925,13 +42922,13 @@
     </row>
     <row r="92" spans="1:21">
       <c r="A92" t="s">
-        <v>4611</v>
+        <v>4609</v>
       </c>
       <c r="B92" t="s">
-        <v>4611</v>
+        <v>4609</v>
       </c>
       <c r="C92" t="s">
-        <v>4610</v>
+        <v>4608</v>
       </c>
       <c r="D92" t="s">
         <v>21</v>
@@ -42940,7 +42937,7 @@
         <v>805</v>
       </c>
       <c r="F92" t="s">
-        <v>4609</v>
+        <v>4607</v>
       </c>
       <c r="G92" t="str">
         <f>Config!$B$4</f>
@@ -42959,42 +42956,42 @@
         <v>2.1999999999999999E-5</v>
       </c>
       <c r="L92" t="s">
-        <v>4606</v>
+        <v>4604</v>
       </c>
       <c r="M92" t="s">
         <v>4362</v>
       </c>
       <c r="N92" t="s">
-        <v>4604</v>
+        <v>4602</v>
       </c>
       <c r="O92" t="s">
         <v>26</v>
       </c>
       <c r="P92" t="s">
-        <v>4605</v>
+        <v>4603</v>
       </c>
       <c r="Q92" t="s">
         <v>4362</v>
       </c>
       <c r="R92" t="s">
-        <v>4608</v>
+        <v>4606</v>
       </c>
       <c r="S92" t="s">
         <v>26</v>
       </c>
       <c r="T92" t="s">
-        <v>4607</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="93" spans="1:21">
       <c r="A93" t="s">
-        <v>4687</v>
+        <v>4668</v>
       </c>
       <c r="B93" t="s">
-        <v>4687</v>
+        <v>4668</v>
       </c>
       <c r="C93" t="s">
-        <v>4688</v>
+        <v>4669</v>
       </c>
       <c r="D93" t="s">
         <v>21</v>
@@ -43022,19 +43019,19 @@
         <v>1.0000000000000002E-6</v>
       </c>
       <c r="L93" t="s">
-        <v>4690</v>
+        <v>4671</v>
       </c>
       <c r="M93" t="s">
-        <v>4692</v>
+        <v>4673</v>
       </c>
       <c r="N93" t="s">
-        <v>4689</v>
+        <v>4670</v>
       </c>
       <c r="O93" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="P93" t="s">
-        <v>4691</v>
+        <v>4672</v>
       </c>
       <c r="U93" s="4"/>
     </row>
@@ -43128,22 +43125,22 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>4653</v>
+        <v>4634</v>
       </c>
       <c r="B2" t="s">
-        <v>4653</v>
+        <v>4634</v>
       </c>
       <c r="C2" t="s">
-        <v>4666</v>
+        <v>4647</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>4528</v>
+        <v>4526</v>
       </c>
       <c r="F2" t="s">
-        <v>4679</v>
+        <v>4660</v>
       </c>
       <c r="G2" t="str">
         <f>Config!$B$5</f>
@@ -43156,57 +43153,57 @@
         <v>464</v>
       </c>
       <c r="J2" t="s">
-        <v>4530</v>
+        <v>4528</v>
       </c>
       <c r="K2" s="4">
         <v>4.7E-7</v>
       </c>
       <c r="L2" t="s">
-        <v>4531</v>
+        <v>4529</v>
       </c>
       <c r="M2" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N2" t="s">
-        <v>4534</v>
+        <v>4532</v>
       </c>
       <c r="O2" t="s">
         <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>4535</v>
+        <v>4533</v>
       </c>
       <c r="Q2" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R2" t="s">
-        <v>4545</v>
+        <v>4543</v>
       </c>
       <c r="S2" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T2" t="s">
-        <v>4549</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>4654</v>
+        <v>4635</v>
       </c>
       <c r="B3" t="s">
-        <v>4654</v>
+        <v>4635</v>
       </c>
       <c r="C3" t="s">
-        <v>4667</v>
+        <v>4648</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>4528</v>
+        <v>4526</v>
       </c>
       <c r="F3" t="s">
-        <v>4680</v>
+        <v>4661</v>
       </c>
       <c r="G3" t="str">
         <f>Config!$B$5</f>
@@ -43219,57 +43216,57 @@
         <v>464</v>
       </c>
       <c r="J3" t="s">
-        <v>4530</v>
+        <v>4528</v>
       </c>
       <c r="K3" s="4">
         <v>6.7999999999999995E-7</v>
       </c>
       <c r="L3" t="s">
-        <v>4531</v>
+        <v>4529</v>
       </c>
       <c r="M3" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N3" t="s">
-        <v>4537</v>
+        <v>4535</v>
       </c>
       <c r="O3" t="s">
         <v>26</v>
       </c>
       <c r="P3" t="s">
-        <v>4536</v>
+        <v>4534</v>
       </c>
       <c r="Q3" t="s">
+        <v>4550</v>
+      </c>
+      <c r="R3" t="s">
+        <v>4551</v>
+      </c>
+      <c r="S3" t="s">
+        <v>4633</v>
+      </c>
+      <c r="T3" t="s">
         <v>4552</v>
-      </c>
-      <c r="R3" t="s">
-        <v>4553</v>
-      </c>
-      <c r="S3" t="s">
-        <v>4635</v>
-      </c>
-      <c r="T3" t="s">
-        <v>4554</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>4655</v>
+        <v>4636</v>
       </c>
       <c r="B4" t="s">
-        <v>4655</v>
+        <v>4636</v>
       </c>
       <c r="C4" t="s">
-        <v>4668</v>
+        <v>4649</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>4528</v>
+        <v>4526</v>
       </c>
       <c r="F4" t="s">
-        <v>4681</v>
+        <v>4662</v>
       </c>
       <c r="G4" t="str">
         <f>Config!$B$5</f>
@@ -43282,57 +43279,57 @@
         <v>464</v>
       </c>
       <c r="J4" t="s">
-        <v>4530</v>
+        <v>4528</v>
       </c>
       <c r="K4" s="4">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="L4" t="s">
-        <v>4531</v>
+        <v>4529</v>
       </c>
       <c r="M4" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N4" t="s">
-        <v>4539</v>
+        <v>4537</v>
       </c>
       <c r="O4" t="s">
         <v>26</v>
       </c>
       <c r="P4" t="s">
-        <v>4538</v>
+        <v>4536</v>
       </c>
       <c r="Q4" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R4" t="s">
-        <v>4555</v>
+        <v>4553</v>
       </c>
       <c r="S4" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T4" t="s">
-        <v>4556</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>4656</v>
+        <v>4637</v>
       </c>
       <c r="B5" t="s">
-        <v>4656</v>
+        <v>4637</v>
       </c>
       <c r="C5" t="s">
-        <v>4669</v>
+        <v>4650</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>4528</v>
+        <v>4526</v>
       </c>
       <c r="F5" t="s">
-        <v>4682</v>
+        <v>4663</v>
       </c>
       <c r="G5" t="str">
         <f>Config!$B$5</f>
@@ -43345,57 +43342,57 @@
         <v>464</v>
       </c>
       <c r="J5" t="s">
-        <v>4530</v>
+        <v>4528</v>
       </c>
       <c r="K5" s="4">
         <v>1.5E-6</v>
       </c>
       <c r="L5" t="s">
+        <v>4529</v>
+      </c>
+      <c r="M5" t="s">
+        <v>4542</v>
+      </c>
+      <c r="N5" t="s">
+        <v>4530</v>
+      </c>
+      <c r="O5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" t="s">
         <v>4531</v>
       </c>
-      <c r="M5" t="s">
-        <v>4544</v>
-      </c>
-      <c r="N5" t="s">
-        <v>4532</v>
-      </c>
-      <c r="O5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" t="s">
-        <v>4533</v>
-      </c>
       <c r="Q5" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R5" t="s">
-        <v>4557</v>
+        <v>4555</v>
       </c>
       <c r="S5" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T5" t="s">
-        <v>4558</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>4657</v>
+        <v>4638</v>
       </c>
       <c r="B6" t="s">
-        <v>4657</v>
+        <v>4638</v>
       </c>
       <c r="C6" t="s">
-        <v>4670</v>
+        <v>4651</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>4528</v>
+        <v>4526</v>
       </c>
       <c r="F6" t="s">
-        <v>4683</v>
+        <v>4664</v>
       </c>
       <c r="G6" t="str">
         <f>Config!$B$5</f>
@@ -43408,57 +43405,57 @@
         <v>464</v>
       </c>
       <c r="J6" t="s">
-        <v>4530</v>
+        <v>4528</v>
       </c>
       <c r="K6" s="4">
         <v>2.2000000000000001E-6</v>
       </c>
       <c r="L6" t="s">
-        <v>4531</v>
+        <v>4529</v>
       </c>
       <c r="M6" t="s">
+        <v>4542</v>
+      </c>
+      <c r="N6" t="s">
+        <v>4538</v>
+      </c>
+      <c r="O6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" t="s">
+        <v>4539</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>4546</v>
+      </c>
+      <c r="R6" t="s">
         <v>4544</v>
       </c>
-      <c r="N6" t="s">
-        <v>4540</v>
-      </c>
-      <c r="O6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P6" t="s">
-        <v>4541</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>4548</v>
-      </c>
-      <c r="R6" t="s">
-        <v>4546</v>
-      </c>
       <c r="S6" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T6" t="s">
-        <v>4551</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>4658</v>
+        <v>4639</v>
       </c>
       <c r="B7" t="s">
-        <v>4658</v>
+        <v>4639</v>
       </c>
       <c r="C7" t="s">
-        <v>4671</v>
+        <v>4652</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>4528</v>
+        <v>4526</v>
       </c>
       <c r="F7" t="s">
-        <v>4686</v>
+        <v>4667</v>
       </c>
       <c r="G7" t="str">
         <f>Config!$B$5</f>
@@ -43471,57 +43468,57 @@
         <v>464</v>
       </c>
       <c r="J7" t="s">
-        <v>4530</v>
+        <v>4528</v>
       </c>
       <c r="K7" s="4">
         <v>4.6999999999999999E-6</v>
       </c>
       <c r="L7" t="s">
-        <v>4531</v>
+        <v>4529</v>
       </c>
       <c r="M7" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N7" t="s">
-        <v>4542</v>
+        <v>4540</v>
       </c>
       <c r="O7" t="s">
         <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>4543</v>
+        <v>4541</v>
       </c>
       <c r="Q7" t="s">
+        <v>4546</v>
+      </c>
+      <c r="R7" t="s">
+        <v>4545</v>
+      </c>
+      <c r="S7" t="s">
+        <v>4633</v>
+      </c>
+      <c r="T7" t="s">
         <v>4548</v>
-      </c>
-      <c r="R7" t="s">
-        <v>4547</v>
-      </c>
-      <c r="S7" t="s">
-        <v>4635</v>
-      </c>
-      <c r="T7" t="s">
-        <v>4550</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>4659</v>
+        <v>4640</v>
       </c>
       <c r="B8" t="s">
-        <v>4659</v>
+        <v>4640</v>
       </c>
       <c r="C8" t="s">
-        <v>4672</v>
+        <v>4653</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>4589</v>
+        <v>4587</v>
       </c>
       <c r="F8" t="s">
-        <v>4685</v>
+        <v>4666</v>
       </c>
       <c r="G8" t="str">
         <f>Config!$B$5</f>
@@ -43534,57 +43531,57 @@
         <v>464</v>
       </c>
       <c r="J8" t="s">
-        <v>4566</v>
+        <v>4564</v>
       </c>
       <c r="K8" s="4">
         <v>2.3999999999999998E-7</v>
       </c>
       <c r="L8" t="s">
-        <v>4581</v>
+        <v>4579</v>
       </c>
       <c r="M8" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N8" t="s">
-        <v>4568</v>
+        <v>4566</v>
       </c>
       <c r="O8" t="s">
         <v>26</v>
       </c>
       <c r="P8" t="s">
-        <v>4567</v>
+        <v>4565</v>
       </c>
       <c r="Q8" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R8" t="s">
-        <v>4559</v>
+        <v>4557</v>
       </c>
       <c r="S8" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T8" t="s">
-        <v>4582</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>4660</v>
+        <v>4641</v>
       </c>
       <c r="B9" t="s">
-        <v>4660</v>
+        <v>4641</v>
       </c>
       <c r="C9" t="s">
-        <v>4673</v>
+        <v>4654</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>4589</v>
+        <v>4587</v>
       </c>
       <c r="F9" t="s">
-        <v>4684</v>
+        <v>4665</v>
       </c>
       <c r="G9" t="str">
         <f>Config!$B$5</f>
@@ -43597,57 +43594,57 @@
         <v>464</v>
       </c>
       <c r="J9" t="s">
-        <v>4566</v>
+        <v>4564</v>
       </c>
       <c r="K9" s="4">
         <v>3.3000000000000002E-7</v>
       </c>
       <c r="L9" t="s">
-        <v>4581</v>
+        <v>4579</v>
       </c>
       <c r="M9" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N9" t="s">
-        <v>4569</v>
+        <v>4567</v>
       </c>
       <c r="O9" t="s">
         <v>26</v>
       </c>
       <c r="P9" t="s">
-        <v>4575</v>
+        <v>4573</v>
       </c>
       <c r="Q9" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R9" t="s">
-        <v>4560</v>
+        <v>4558</v>
       </c>
       <c r="S9" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T9" t="s">
-        <v>4585</v>
+        <v>4583</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>4661</v>
+        <v>4642</v>
       </c>
       <c r="B10" t="s">
-        <v>4661</v>
+        <v>4642</v>
       </c>
       <c r="C10" t="s">
-        <v>4674</v>
+        <v>4655</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>4589</v>
+        <v>4587</v>
       </c>
       <c r="F10" t="s">
-        <v>4679</v>
+        <v>4660</v>
       </c>
       <c r="G10" t="str">
         <f>Config!$B$5</f>
@@ -43660,57 +43657,57 @@
         <v>464</v>
       </c>
       <c r="J10" t="s">
-        <v>4566</v>
+        <v>4564</v>
       </c>
       <c r="K10" s="4">
         <v>4.7E-7</v>
       </c>
       <c r="L10" t="s">
-        <v>4581</v>
+        <v>4579</v>
       </c>
       <c r="M10" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N10" t="s">
-        <v>4570</v>
+        <v>4568</v>
       </c>
       <c r="O10" t="s">
         <v>26</v>
       </c>
       <c r="P10" t="s">
-        <v>4576</v>
+        <v>4574</v>
       </c>
       <c r="Q10" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R10" t="s">
-        <v>4561</v>
+        <v>4559</v>
       </c>
       <c r="S10" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T10" t="s">
-        <v>4586</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>4662</v>
+        <v>4643</v>
       </c>
       <c r="B11" t="s">
-        <v>4662</v>
+        <v>4643</v>
       </c>
       <c r="C11" t="s">
-        <v>4675</v>
+        <v>4656</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>4589</v>
+        <v>4587</v>
       </c>
       <c r="F11" t="s">
-        <v>4680</v>
+        <v>4661</v>
       </c>
       <c r="G11" t="str">
         <f>Config!$B$5</f>
@@ -43723,57 +43720,57 @@
         <v>464</v>
       </c>
       <c r="J11" t="s">
-        <v>4566</v>
+        <v>4564</v>
       </c>
       <c r="K11" s="4">
         <v>6.7999999999999995E-7</v>
       </c>
       <c r="L11" t="s">
-        <v>4581</v>
+        <v>4579</v>
       </c>
       <c r="M11" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N11" t="s">
-        <v>4571</v>
+        <v>4569</v>
       </c>
       <c r="O11" t="s">
         <v>26</v>
       </c>
       <c r="P11" t="s">
-        <v>4577</v>
+        <v>4575</v>
       </c>
       <c r="Q11" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R11" t="s">
-        <v>4562</v>
+        <v>4560</v>
       </c>
       <c r="S11" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T11" t="s">
-        <v>4587</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>4663</v>
+        <v>4644</v>
       </c>
       <c r="B12" t="s">
-        <v>4663</v>
+        <v>4644</v>
       </c>
       <c r="C12" t="s">
-        <v>4676</v>
+        <v>4657</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>4589</v>
+        <v>4587</v>
       </c>
       <c r="F12" t="s">
-        <v>4681</v>
+        <v>4662</v>
       </c>
       <c r="G12" t="str">
         <f>Config!$B$5</f>
@@ -43786,57 +43783,57 @@
         <v>464</v>
       </c>
       <c r="J12" t="s">
-        <v>4566</v>
+        <v>4564</v>
       </c>
       <c r="K12" s="4">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="L12" t="s">
-        <v>4581</v>
+        <v>4579</v>
       </c>
       <c r="M12" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N12" t="s">
-        <v>4572</v>
+        <v>4570</v>
       </c>
       <c r="O12" t="s">
         <v>26</v>
       </c>
       <c r="P12" t="s">
-        <v>4578</v>
+        <v>4576</v>
       </c>
       <c r="Q12" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R12" t="s">
-        <v>4563</v>
+        <v>4561</v>
       </c>
       <c r="S12" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T12" t="s">
-        <v>4588</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>4664</v>
+        <v>4645</v>
       </c>
       <c r="B13" t="s">
-        <v>4664</v>
+        <v>4645</v>
       </c>
       <c r="C13" t="s">
-        <v>4677</v>
+        <v>4658</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>4589</v>
+        <v>4587</v>
       </c>
       <c r="F13" t="s">
-        <v>4682</v>
+        <v>4663</v>
       </c>
       <c r="G13" t="str">
         <f>Config!$B$5</f>
@@ -43849,57 +43846,57 @@
         <v>464</v>
       </c>
       <c r="J13" t="s">
-        <v>4566</v>
+        <v>4564</v>
       </c>
       <c r="K13" s="4">
         <v>1.5E-6</v>
       </c>
       <c r="L13" t="s">
+        <v>4579</v>
+      </c>
+      <c r="M13" t="s">
+        <v>4542</v>
+      </c>
+      <c r="N13" t="s">
+        <v>4571</v>
+      </c>
+      <c r="O13" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" t="s">
+        <v>4577</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>4546</v>
+      </c>
+      <c r="R13" t="s">
+        <v>4562</v>
+      </c>
+      <c r="S13" t="s">
+        <v>4633</v>
+      </c>
+      <c r="T13" t="s">
         <v>4581</v>
-      </c>
-      <c r="M13" t="s">
-        <v>4544</v>
-      </c>
-      <c r="N13" t="s">
-        <v>4573</v>
-      </c>
-      <c r="O13" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" t="s">
-        <v>4579</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>4548</v>
-      </c>
-      <c r="R13" t="s">
-        <v>4564</v>
-      </c>
-      <c r="S13" t="s">
-        <v>4635</v>
-      </c>
-      <c r="T13" t="s">
-        <v>4583</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>4665</v>
+        <v>4646</v>
       </c>
       <c r="B14" t="s">
-        <v>4665</v>
+        <v>4646</v>
       </c>
       <c r="C14" t="s">
-        <v>4678</v>
+        <v>4659</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>4589</v>
+        <v>4587</v>
       </c>
       <c r="F14" t="s">
-        <v>4683</v>
+        <v>4664</v>
       </c>
       <c r="G14" t="str">
         <f>Config!$B$5</f>
@@ -43912,37 +43909,37 @@
         <v>464</v>
       </c>
       <c r="J14" t="s">
-        <v>4566</v>
+        <v>4564</v>
       </c>
       <c r="K14" s="4">
         <v>2.2000000000000001E-6</v>
       </c>
       <c r="L14" t="s">
-        <v>4581</v>
+        <v>4579</v>
       </c>
       <c r="M14" t="s">
-        <v>4544</v>
+        <v>4542</v>
       </c>
       <c r="N14" t="s">
-        <v>4574</v>
+        <v>4572</v>
       </c>
       <c r="O14" t="s">
         <v>26</v>
       </c>
       <c r="P14" t="s">
-        <v>4580</v>
+        <v>4578</v>
       </c>
       <c r="Q14" t="s">
-        <v>4548</v>
+        <v>4546</v>
       </c>
       <c r="R14" t="s">
-        <v>4565</v>
+        <v>4563</v>
       </c>
       <c r="S14" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T14" t="s">
-        <v>4584</v>
+        <v>4582</v>
       </c>
     </row>
   </sheetData>
@@ -44032,16 +44029,16 @@
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>4693</v>
+        <v>4674</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>4694</v>
+        <v>4675</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>4695</v>
+        <v>4676</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>4696</v>
+        <v>4677</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -44106,16 +44103,16 @@
         <v>2722</v>
       </c>
       <c r="U2" t="s">
-        <v>4697</v>
+        <v>4678</v>
       </c>
       <c r="V2" t="s">
         <v>2711</v>
       </c>
       <c r="W2" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="X2" t="s">
-        <v>4698</v>
+        <v>4679</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -69795,7 +69792,7 @@
         <v>2917</v>
       </c>
       <c r="L488" t="s">
-        <v>4636</v>
+        <v>4689</v>
       </c>
       <c r="M488" t="s">
         <v>2701</v>
@@ -69804,7 +69801,7 @@
         <v>4296</v>
       </c>
       <c r="O488" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="P488" t="s">
         <v>4298</v>
@@ -69816,7 +69813,7 @@
         <v>4301</v>
       </c>
       <c r="S488" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T488" t="s">
         <v>4299</v>
@@ -69857,13 +69854,13 @@
         <v>2967</v>
       </c>
       <c r="L489" t="s">
-        <v>4636</v>
+        <v>4689</v>
       </c>
       <c r="M489" t="s">
         <v>4300</v>
       </c>
       <c r="O489" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="P489" t="s">
         <v>4303</v>
@@ -69875,7 +69872,7 @@
         <v>4302</v>
       </c>
       <c r="S489" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T489" t="s">
         <v>4304</v>
@@ -69937,7 +69934,7 @@
         <v>4353</v>
       </c>
       <c r="S490" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T490" t="s">
         <v>4354</v>
@@ -69999,7 +69996,7 @@
         <v>4348</v>
       </c>
       <c r="S491" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T491" t="s">
         <v>4350</v>
@@ -70061,7 +70058,7 @@
         <v>4352</v>
       </c>
       <c r="S492" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T492" t="s">
         <v>4351</v>
@@ -70123,7 +70120,7 @@
         <v>4357</v>
       </c>
       <c r="S493" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T493" t="s">
         <v>4358</v>
@@ -70185,7 +70182,7 @@
         <v>4356</v>
       </c>
       <c r="S494" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="T494" t="s">
         <v>4355</v>
@@ -70193,22 +70190,22 @@
     </row>
     <row r="495" spans="1:20">
       <c r="A495" t="s">
+        <v>4482</v>
+      </c>
+      <c r="B495" t="s">
+        <v>4482</v>
+      </c>
+      <c r="C495" t="s">
         <v>4484</v>
       </c>
-      <c r="B495" t="s">
-        <v>4484</v>
-      </c>
-      <c r="C495" t="s">
+      <c r="D495" t="s">
+        <v>4485</v>
+      </c>
+      <c r="E495" t="s">
         <v>4486</v>
       </c>
-      <c r="D495" t="s">
+      <c r="F495" t="s">
         <v>4487</v>
-      </c>
-      <c r="E495" t="s">
-        <v>4488</v>
-      </c>
-      <c r="F495" t="s">
-        <v>4489</v>
       </c>
       <c r="G495" t="s">
         <v>2715</v>
@@ -70220,37 +70217,37 @@
         <v>2716</v>
       </c>
       <c r="J495" t="s">
-        <v>4485</v>
+        <v>4483</v>
       </c>
       <c r="K495" t="s">
         <v>2978</v>
       </c>
       <c r="L495" t="s">
+        <v>4488</v>
+      </c>
+      <c r="M495" t="s">
+        <v>4489</v>
+      </c>
+      <c r="N495" t="s">
+        <v>4482</v>
+      </c>
+      <c r="O495" t="s">
+        <v>26</v>
+      </c>
+      <c r="P495" t="s">
         <v>4490</v>
       </c>
-      <c r="M495" t="s">
+      <c r="Q495" t="s">
         <v>4491</v>
       </c>
-      <c r="N495" t="s">
-        <v>4484</v>
-      </c>
-      <c r="O495" t="s">
-        <v>26</v>
-      </c>
-      <c r="P495" t="s">
+      <c r="R495" t="s">
+        <v>4482</v>
+      </c>
+      <c r="S495" t="s">
+        <v>4633</v>
+      </c>
+      <c r="T495" t="s">
         <v>4492</v>
-      </c>
-      <c r="Q495" t="s">
-        <v>4493</v>
-      </c>
-      <c r="R495" t="s">
-        <v>4484</v>
-      </c>
-      <c r="S495" t="s">
-        <v>4635</v>
-      </c>
-      <c r="T495" t="s">
-        <v>4494</v>
       </c>
     </row>
   </sheetData>
@@ -70339,22 +70336,22 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>4500</v>
+        <v>4498</v>
       </c>
       <c r="B2" t="s">
-        <v>4500</v>
+        <v>4498</v>
       </c>
       <c r="C2" t="s">
-        <v>4501</v>
+        <v>4499</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>4503</v>
+        <v>4501</v>
       </c>
       <c r="H2" t="s">
-        <v>4502</v>
+        <v>4500</v>
       </c>
     </row>
   </sheetData>
@@ -70439,110 +70436,110 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
+        <v>4503</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4503</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4504</v>
+      </c>
+      <c r="D2" t="s">
         <v>4505</v>
       </c>
-      <c r="B2" t="s">
-        <v>4505</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>4506</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4507</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4508</v>
       </c>
       <c r="G2" t="str">
         <f>Config!$B$6</f>
         <v>SCH/Logic_IEC.SchLib</v>
       </c>
       <c r="H2" t="s">
-        <v>4527</v>
+        <v>4525</v>
       </c>
       <c r="M2" t="s">
+        <v>4505</v>
+      </c>
+      <c r="N2" t="s">
         <v>4507</v>
       </c>
-      <c r="N2" t="s">
-        <v>4509</v>
-      </c>
       <c r="O2" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="P2" t="s">
-        <v>4510</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
+        <v>4509</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4509</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4510</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4472</v>
+      </c>
+      <c r="E3" t="s">
         <v>4511</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4511</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4512</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4474</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4513</v>
       </c>
       <c r="G3" t="str">
         <f>Config!$B$6</f>
         <v>SCH/Logic_IEC.SchLib</v>
       </c>
       <c r="H3" t="s">
+        <v>4512</v>
+      </c>
+      <c r="M3" t="s">
+        <v>4472</v>
+      </c>
+      <c r="N3" t="s">
+        <v>4513</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4633</v>
+      </c>
+      <c r="P3" t="s">
         <v>4514</v>
-      </c>
-      <c r="M3" t="s">
-        <v>4474</v>
-      </c>
-      <c r="N3" t="s">
-        <v>4515</v>
-      </c>
-      <c r="O3" t="s">
-        <v>4635</v>
-      </c>
-      <c r="P3" t="s">
-        <v>4516</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
+        <v>4516</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4516</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4517</v>
+      </c>
+      <c r="D4" t="s">
         <v>4518</v>
       </c>
-      <c r="B4" t="s">
-        <v>4518</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>4519</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4520</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4521</v>
       </c>
       <c r="G4" t="str">
         <f>Config!$B$6</f>
         <v>SCH/Logic_IEC.SchLib</v>
       </c>
       <c r="H4" t="s">
-        <v>4525</v>
+        <v>4523</v>
       </c>
       <c r="M4" t="s">
-        <v>4520</v>
+        <v>4518</v>
       </c>
       <c r="N4" t="s">
-        <v>4517</v>
+        <v>4515</v>
       </c>
       <c r="O4" t="s">
-        <v>4635</v>
+        <v>4633</v>
       </c>
       <c r="P4" t="s">
-        <v>4526</v>
+        <v>4524</v>
       </c>
     </row>
   </sheetData>
@@ -70627,46 +70624,46 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
+        <v>4415</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4415</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4416</v>
+      </c>
+      <c r="D2" t="s">
         <v>4417</v>
       </c>
-      <c r="B2" t="s">
-        <v>4417</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>4418</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>4419</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>4415</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4502</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4415</v>
+      </c>
+      <c r="L2" t="s">
         <v>4420</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M2" t="s">
+        <v>4422</v>
+      </c>
+      <c r="N2" t="s">
+        <v>4415</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4633</v>
+      </c>
+      <c r="P2" t="s">
         <v>4421</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4417</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4504</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4417</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4422</v>
-      </c>
-      <c r="M2" t="s">
-        <v>4424</v>
-      </c>
-      <c r="N2" t="s">
-        <v>4417</v>
-      </c>
-      <c r="O2" t="s">
-        <v>4635</v>
-      </c>
-      <c r="P2" t="s">
-        <v>4423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SOT-363 and 2X4 pin header added
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6A5C5A-CECD-47D0-BB40-69868DF4DF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D1F135-194B-4AAA-81DA-C6C5F0B0AF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="17325" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="6" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16495" uniqueCount="4706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16503" uniqueCount="4711">
   <si>
     <t>Part Number</t>
   </si>
@@ -14164,6 +14164,21 @@
   </si>
   <si>
     <t>https://datasheet.lcsc.com/lcsc/1809211431_AnBon-AS2302_C232266.pdf</t>
+  </si>
+  <si>
+    <t>SOP127P600X155-16</t>
+  </si>
+  <si>
+    <t>SOP127P600X155-14</t>
+  </si>
+  <si>
+    <t>SOT65P210X95-6</t>
+  </si>
+  <si>
+    <t>PCB/Header_254.PcbLib</t>
+  </si>
+  <si>
+    <t>HEAD_254_2X4</t>
   </si>
 </sst>
 </file>
@@ -14568,7 +14583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E41C041-8921-4AFD-BA29-DDEA3EB18923}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -14864,11 +14879,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8992C59-F5E3-466D-8132-19915B114D9C}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -70263,11 +70278,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05348336-C131-49E6-98A6-4A6B8B6DDA7F}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -70352,6 +70367,12 @@
       </c>
       <c r="H2" t="s">
         <v>4500</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4709</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4710</v>
       </c>
     </row>
   </sheetData>
@@ -70367,7 +70388,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -70457,6 +70478,12 @@
       <c r="H2" t="s">
         <v>4525</v>
       </c>
+      <c r="I2" t="s">
+        <v>4445</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4706</v>
+      </c>
       <c r="M2" t="s">
         <v>4505</v>
       </c>
@@ -70493,6 +70520,12 @@
       <c r="H3" t="s">
         <v>4512</v>
       </c>
+      <c r="I3" t="s">
+        <v>4444</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4708</v>
+      </c>
       <c r="M3" t="s">
         <v>4472</v>
       </c>
@@ -70528,6 +70561,12 @@
       </c>
       <c r="H4" t="s">
         <v>4523</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4445</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4707</v>
       </c>
       <c r="M4" t="s">
         <v>4518</v>

</xml_diff>

<commit_message>
WS2813B-B added, SOP14 and SOP16 component reference corrected
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D1F135-194B-4AAA-81DA-C6C5F0B0AF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA44B61-DF9B-48B2-B506-0F15B60DDDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="6" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16503" uniqueCount="4711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16517" uniqueCount="4718">
   <si>
     <t>Part Number</t>
   </si>
@@ -14179,6 +14179,27 @@
   </si>
   <si>
     <t>HEAD_254_2X4</t>
+  </si>
+  <si>
+    <t>WS2813B-B</t>
+  </si>
+  <si>
+    <t>WS2813_NC</t>
+  </si>
+  <si>
+    <t>WS2813_BO</t>
+  </si>
+  <si>
+    <t>WS2813_VCC</t>
+  </si>
+  <si>
+    <t>LEDM5050X165-7</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1809261040_Worldsemi-WS2813B-B_C114592.pdf</t>
+  </si>
+  <si>
+    <t>C114592</t>
   </si>
 </sst>
 </file>
@@ -14877,13 +14898,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8992C59-F5E3-466D-8132-19915B114D9C}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -14990,7 +15011,7 @@
         <v>4444</v>
       </c>
       <c r="I2" t="s">
-        <v>2696</v>
+        <v>4627</v>
       </c>
       <c r="J2" t="s">
         <v>4690</v>
@@ -15113,7 +15134,7 @@
         <v>2697</v>
       </c>
       <c r="G5" t="s">
-        <v>3584</v>
+        <v>4712</v>
       </c>
       <c r="H5" t="s">
         <v>3914</v>
@@ -15157,7 +15178,7 @@
         <v>2697</v>
       </c>
       <c r="G6" t="s">
-        <v>3911</v>
+        <v>4713</v>
       </c>
       <c r="H6" t="s">
         <v>3914</v>
@@ -15183,10 +15204,10 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>3903</v>
+        <v>4711</v>
       </c>
       <c r="B7" t="s">
-        <v>3903</v>
+        <v>4711</v>
       </c>
       <c r="C7" t="s">
         <v>3905</v>
@@ -15195,86 +15216,86 @@
         <v>3907</v>
       </c>
       <c r="E7" t="s">
-        <v>3909</v>
+        <v>3908</v>
       </c>
       <c r="F7" t="s">
         <v>2697</v>
       </c>
       <c r="G7" t="s">
-        <v>3911</v>
+        <v>4714</v>
       </c>
       <c r="H7" t="s">
         <v>3914</v>
       </c>
       <c r="I7" t="s">
-        <v>4285</v>
+        <v>4715</v>
       </c>
       <c r="J7" t="s">
-        <v>4695</v>
+        <v>4716</v>
       </c>
       <c r="K7" t="s">
         <v>3907</v>
       </c>
       <c r="L7" t="s">
-        <v>4287</v>
+        <v>4711</v>
       </c>
       <c r="M7" t="s">
         <v>4633</v>
       </c>
       <c r="N7" t="s">
-        <v>4289</v>
+        <v>4717</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>3912</v>
+        <v>3903</v>
       </c>
       <c r="B8" t="s">
-        <v>3912</v>
+        <v>3903</v>
       </c>
       <c r="C8" t="s">
-        <v>3904</v>
+        <v>3905</v>
       </c>
       <c r="D8" t="s">
         <v>3907</v>
       </c>
       <c r="E8" t="s">
-        <v>3908</v>
+        <v>3909</v>
       </c>
       <c r="F8" t="s">
         <v>2697</v>
       </c>
       <c r="G8" t="s">
-        <v>3913</v>
+        <v>3911</v>
       </c>
       <c r="H8" t="s">
         <v>3914</v>
       </c>
       <c r="I8" t="s">
-        <v>4283</v>
+        <v>4285</v>
       </c>
       <c r="J8" t="s">
-        <v>4696</v>
+        <v>4695</v>
       </c>
       <c r="K8" t="s">
         <v>3907</v>
       </c>
       <c r="L8" t="s">
-        <v>4290</v>
+        <v>4287</v>
       </c>
       <c r="M8" t="s">
         <v>4633</v>
       </c>
       <c r="N8" t="s">
-        <v>4291</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>3910</v>
+        <v>3912</v>
       </c>
       <c r="B9" t="s">
-        <v>3910</v>
+        <v>3912</v>
       </c>
       <c r="C9" t="s">
         <v>3904</v>
@@ -15298,27 +15319,27 @@
         <v>4283</v>
       </c>
       <c r="J9" t="s">
-        <v>4697</v>
+        <v>4696</v>
       </c>
       <c r="K9" t="s">
         <v>3907</v>
       </c>
       <c r="L9" t="s">
-        <v>3910</v>
+        <v>4290</v>
       </c>
       <c r="M9" t="s">
         <v>4633</v>
       </c>
       <c r="N9" t="s">
-        <v>4292</v>
+        <v>4291</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>3906</v>
+        <v>3910</v>
       </c>
       <c r="B10" t="s">
-        <v>3906</v>
+        <v>3910</v>
       </c>
       <c r="C10" t="s">
         <v>3904</v>
@@ -15327,7 +15348,7 @@
         <v>3907</v>
       </c>
       <c r="E10" t="s">
-        <v>3909</v>
+        <v>3908</v>
       </c>
       <c r="F10" t="s">
         <v>2697</v>
@@ -15339,177 +15360,165 @@
         <v>3914</v>
       </c>
       <c r="I10" t="s">
-        <v>4284</v>
+        <v>4283</v>
       </c>
       <c r="J10" t="s">
-        <v>4698</v>
+        <v>4697</v>
       </c>
       <c r="K10" t="s">
         <v>3907</v>
       </c>
       <c r="L10" t="s">
-        <v>4294</v>
+        <v>3910</v>
       </c>
       <c r="M10" t="s">
         <v>4633</v>
       </c>
       <c r="N10" t="s">
-        <v>4293</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>4438</v>
+        <v>3906</v>
       </c>
       <c r="B11" t="s">
-        <v>4438</v>
+        <v>3906</v>
       </c>
       <c r="C11" t="s">
-        <v>4439</v>
+        <v>3904</v>
       </c>
       <c r="D11" t="s">
-        <v>4443</v>
+        <v>3907</v>
       </c>
       <c r="E11" t="s">
-        <v>4440</v>
+        <v>3909</v>
       </c>
       <c r="F11" t="s">
         <v>2697</v>
       </c>
       <c r="G11" t="s">
-        <v>4438</v>
+        <v>3913</v>
       </c>
       <c r="H11" t="s">
-        <v>4444</v>
+        <v>3914</v>
       </c>
       <c r="I11" t="s">
-        <v>2696</v>
+        <v>4284</v>
       </c>
       <c r="J11" t="s">
-        <v>4699</v>
+        <v>4698</v>
       </c>
       <c r="K11" t="s">
-        <v>4443</v>
+        <v>3907</v>
       </c>
       <c r="L11" t="s">
-        <v>4441</v>
+        <v>4294</v>
       </c>
       <c r="M11" t="s">
         <v>4633</v>
       </c>
-      <c r="N11" s="8" t="s">
-        <v>4442</v>
+      <c r="N11" t="s">
+        <v>4293</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>4446</v>
+        <v>4438</v>
       </c>
       <c r="B12" t="s">
-        <v>4446</v>
+        <v>4438</v>
       </c>
       <c r="C12" t="s">
-        <v>4448</v>
+        <v>4439</v>
       </c>
       <c r="D12" t="s">
-        <v>4447</v>
+        <v>4443</v>
       </c>
       <c r="E12" t="s">
-        <v>4449</v>
+        <v>4440</v>
       </c>
       <c r="F12" t="s">
         <v>2697</v>
       </c>
       <c r="G12" t="s">
-        <v>4451</v>
+        <v>4438</v>
       </c>
       <c r="H12" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
       <c r="I12" t="s">
-        <v>4452</v>
+        <v>2696</v>
       </c>
       <c r="J12" t="s">
-        <v>4700</v>
+        <v>4699</v>
       </c>
       <c r="K12" t="s">
-        <v>4447</v>
+        <v>4443</v>
       </c>
       <c r="L12" t="s">
-        <v>4446</v>
+        <v>4441</v>
       </c>
       <c r="M12" t="s">
         <v>4633</v>
       </c>
-      <c r="N12" t="s">
-        <v>4450</v>
+      <c r="N12" s="8" t="s">
+        <v>4442</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>4453</v>
+        <v>4446</v>
       </c>
       <c r="B13" t="s">
-        <v>4453</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>4454</v>
+        <v>4446</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4448</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>4447</v>
       </c>
       <c r="E13" t="s">
-        <v>4440</v>
+        <v>4449</v>
       </c>
       <c r="F13" t="s">
         <v>2697</v>
       </c>
       <c r="G13" t="s">
-        <v>4455</v>
+        <v>4451</v>
       </c>
       <c r="H13" t="s">
-        <v>4444</v>
+        <v>4445</v>
       </c>
       <c r="I13" t="s">
-        <v>2696</v>
+        <v>4452</v>
       </c>
       <c r="J13" t="s">
-        <v>4458</v>
+        <v>4700</v>
       </c>
       <c r="K13" t="s">
-        <v>4457</v>
+        <v>4447</v>
       </c>
       <c r="L13" t="s">
-        <v>4453</v>
+        <v>4446</v>
       </c>
       <c r="M13" t="s">
-        <v>26</v>
+        <v>4633</v>
       </c>
       <c r="N13" t="s">
-        <v>4456</v>
-      </c>
-      <c r="O13" t="s">
-        <v>4459</v>
-      </c>
-      <c r="P13" t="s">
-        <v>4453</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>4633</v>
-      </c>
-      <c r="R13" t="s">
-        <v>4460</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>4461</v>
+        <v>4453</v>
       </c>
       <c r="B14" t="s">
-        <v>4461</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4466</v>
+        <v>4453</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>4454</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -15521,7 +15530,7 @@
         <v>2697</v>
       </c>
       <c r="G14" t="s">
-        <v>4465</v>
+        <v>4455</v>
       </c>
       <c r="H14" t="s">
         <v>4444</v>
@@ -15530,42 +15539,42 @@
         <v>2696</v>
       </c>
       <c r="J14" t="s">
-        <v>4464</v>
+        <v>4458</v>
       </c>
       <c r="K14" t="s">
-        <v>4463</v>
+        <v>4457</v>
       </c>
       <c r="L14" t="s">
-        <v>4461</v>
+        <v>4453</v>
       </c>
       <c r="M14" t="s">
         <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>4462</v>
+        <v>4456</v>
       </c>
       <c r="O14" t="s">
-        <v>4467</v>
+        <v>4459</v>
       </c>
       <c r="P14" t="s">
-        <v>4461</v>
+        <v>4453</v>
       </c>
       <c r="Q14" t="s">
         <v>4633</v>
       </c>
       <c r="R14" t="s">
-        <v>4468</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>4469</v>
+        <v>4461</v>
       </c>
       <c r="B15" t="s">
-        <v>4469</v>
+        <v>4461</v>
       </c>
       <c r="C15" t="s">
-        <v>4470</v>
+        <v>4466</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
@@ -15577,7 +15586,7 @@
         <v>2697</v>
       </c>
       <c r="G15" t="s">
-        <v>4455</v>
+        <v>4465</v>
       </c>
       <c r="H15" t="s">
         <v>4444</v>
@@ -15586,30 +15595,42 @@
         <v>2696</v>
       </c>
       <c r="J15" t="s">
-        <v>4471</v>
+        <v>4464</v>
       </c>
       <c r="K15" t="s">
-        <v>4472</v>
+        <v>4463</v>
       </c>
       <c r="L15" t="s">
-        <v>4474</v>
+        <v>4461</v>
       </c>
       <c r="M15" t="s">
         <v>26</v>
       </c>
       <c r="N15" t="s">
-        <v>4473</v>
+        <v>4462</v>
+      </c>
+      <c r="O15" t="s">
+        <v>4467</v>
+      </c>
+      <c r="P15" t="s">
+        <v>4461</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>4633</v>
+      </c>
+      <c r="R15" t="s">
+        <v>4468</v>
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16">
-        <v>2302</v>
+      <c r="A16" t="s">
+        <v>4469</v>
       </c>
       <c r="B16" t="s">
-        <v>4495</v>
+        <v>4469</v>
       </c>
       <c r="C16" t="s">
-        <v>4476</v>
+        <v>4470</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -15627,45 +15648,33 @@
         <v>4444</v>
       </c>
       <c r="I16" t="s">
-        <v>4452</v>
+        <v>2696</v>
       </c>
       <c r="J16" t="s">
-        <v>4701</v>
+        <v>4471</v>
       </c>
       <c r="K16" t="s">
-        <v>4477</v>
+        <v>4472</v>
       </c>
       <c r="L16" t="s">
-        <v>4475</v>
+        <v>4474</v>
       </c>
       <c r="M16" t="s">
-        <v>4633</v>
+        <v>26</v>
       </c>
       <c r="N16" t="s">
-        <v>4478</v>
-      </c>
-      <c r="O16" t="s">
-        <v>4480</v>
-      </c>
-      <c r="P16" t="s">
-        <v>4479</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>4633</v>
-      </c>
-      <c r="R16" t="s">
-        <v>4481</v>
+        <v>4473</v>
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" t="s">
-        <v>4496</v>
+      <c r="A17">
+        <v>2302</v>
       </c>
       <c r="B17" t="s">
-        <v>4496</v>
+        <v>4495</v>
       </c>
       <c r="C17" t="s">
-        <v>4493</v>
+        <v>4476</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
@@ -15677,185 +15686,197 @@
         <v>2697</v>
       </c>
       <c r="G17" t="s">
-        <v>4465</v>
+        <v>4455</v>
       </c>
       <c r="H17" t="s">
         <v>4444</v>
       </c>
       <c r="I17" t="s">
-        <v>2696</v>
+        <v>4452</v>
       </c>
       <c r="J17" t="s">
-        <v>4702</v>
+        <v>4701</v>
       </c>
       <c r="K17" t="s">
-        <v>4497</v>
+        <v>4477</v>
       </c>
       <c r="L17" t="s">
-        <v>4496</v>
+        <v>4475</v>
       </c>
       <c r="M17" t="s">
         <v>4633</v>
       </c>
-      <c r="N17" s="8" t="s">
-        <v>4494</v>
+      <c r="N17" t="s">
+        <v>4478</v>
+      </c>
+      <c r="O17" t="s">
+        <v>4480</v>
+      </c>
+      <c r="P17" t="s">
+        <v>4479</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>4633</v>
+      </c>
+      <c r="R17" t="s">
+        <v>4481</v>
       </c>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>4591</v>
+        <v>4496</v>
       </c>
       <c r="B18" t="s">
-        <v>4591</v>
+        <v>4496</v>
       </c>
       <c r="C18" t="s">
-        <v>4590</v>
+        <v>4493</v>
       </c>
       <c r="D18" t="s">
-        <v>4588</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>4594</v>
+        <v>4440</v>
       </c>
       <c r="F18" t="s">
         <v>2697</v>
       </c>
       <c r="G18" t="s">
-        <v>4591</v>
+        <v>4465</v>
       </c>
       <c r="H18" t="s">
         <v>4444</v>
       </c>
       <c r="I18" t="s">
-        <v>4595</v>
+        <v>2696</v>
       </c>
       <c r="J18" t="s">
-        <v>4593</v>
+        <v>4702</v>
       </c>
       <c r="K18" t="s">
+        <v>4497</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4496</v>
+      </c>
+      <c r="M18" t="s">
+        <v>4633</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>4494</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
+        <v>4591</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4591</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4590</v>
+      </c>
+      <c r="D19" t="s">
         <v>4588</v>
       </c>
-      <c r="L18" t="s">
-        <v>4591</v>
-      </c>
-      <c r="M18" t="s">
-        <v>26</v>
-      </c>
-      <c r="N18" t="s">
-        <v>4592</v>
-      </c>
-      <c r="O18" t="s">
-        <v>4588</v>
-      </c>
-      <c r="P18" t="s">
-        <v>4591</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>4633</v>
-      </c>
-      <c r="R18" s="8" t="s">
-        <v>4589</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="8" t="s">
-        <v>4600</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>4600</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4601</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4598</v>
-      </c>
       <c r="E19" t="s">
-        <v>4626</v>
+        <v>4594</v>
       </c>
       <c r="F19" t="s">
         <v>2697</v>
       </c>
       <c r="G19" t="s">
-        <v>4600</v>
+        <v>4591</v>
       </c>
       <c r="H19" t="s">
         <v>4444</v>
       </c>
       <c r="I19" t="s">
-        <v>4599</v>
+        <v>4595</v>
       </c>
       <c r="J19" t="s">
-        <v>4703</v>
+        <v>4593</v>
       </c>
       <c r="K19" t="s">
-        <v>4598</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>4596</v>
+        <v>4588</v>
+      </c>
+      <c r="L19" t="s">
+        <v>4591</v>
       </c>
       <c r="M19" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" t="s">
+        <v>4592</v>
+      </c>
+      <c r="O19" t="s">
+        <v>4588</v>
+      </c>
+      <c r="P19" t="s">
+        <v>4591</v>
+      </c>
+      <c r="Q19" t="s">
         <v>4633</v>
       </c>
-      <c r="N19" s="8" t="s">
-        <v>4597</v>
+      <c r="R19" s="8" t="s">
+        <v>4589</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="8" t="s">
-        <v>4624</v>
+        <v>4600</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>4624</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>4625</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>21</v>
+        <v>4600</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4601</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4598</v>
       </c>
       <c r="E20" t="s">
-        <v>4440</v>
+        <v>4626</v>
       </c>
       <c r="F20" t="s">
         <v>2697</v>
       </c>
       <c r="G20" t="s">
-        <v>4455</v>
+        <v>4600</v>
       </c>
       <c r="H20" t="s">
         <v>4444</v>
       </c>
       <c r="I20" t="s">
-        <v>2696</v>
+        <v>4599</v>
       </c>
       <c r="J20" t="s">
-        <v>4704</v>
+        <v>4703</v>
       </c>
       <c r="K20" t="s">
-        <v>2709</v>
-      </c>
-      <c r="L20" t="s">
-        <v>2709</v>
+        <v>4598</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>4596</v>
       </c>
       <c r="M20" t="s">
         <v>4633</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>4623</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" t="s">
-        <v>4628</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4628</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4629</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="A21" s="8" t="s">
+        <v>4624</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>4624</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>4625</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E21" t="s">
@@ -15874,45 +15895,33 @@
         <v>2696</v>
       </c>
       <c r="J21" t="s">
-        <v>4705</v>
+        <v>4704</v>
       </c>
       <c r="K21" t="s">
-        <v>4457</v>
+        <v>2709</v>
       </c>
       <c r="L21" t="s">
-        <v>4628</v>
+        <v>2709</v>
       </c>
       <c r="M21" t="s">
-        <v>26</v>
-      </c>
-      <c r="N21" t="s">
-        <v>4630</v>
-      </c>
-      <c r="O21" t="s">
-        <v>4631</v>
-      </c>
-      <c r="P21" t="s">
-        <v>4628</v>
-      </c>
-      <c r="Q21" t="s">
         <v>4633</v>
       </c>
-      <c r="R21" t="s">
-        <v>4632</v>
+      <c r="N21" s="8" t="s">
+        <v>4623</v>
       </c>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
-        <v>4687</v>
+        <v>4628</v>
       </c>
       <c r="B22" t="s">
-        <v>4687</v>
+        <v>4628</v>
       </c>
       <c r="C22" t="s">
-        <v>4682</v>
+        <v>4629</v>
       </c>
       <c r="D22" t="s">
-        <v>4686</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
         <v>4440</v>
@@ -15921,7 +15930,7 @@
         <v>2697</v>
       </c>
       <c r="G22" t="s">
-        <v>4680</v>
+        <v>4455</v>
       </c>
       <c r="H22" t="s">
         <v>4444</v>
@@ -15930,25 +15939,82 @@
         <v>2696</v>
       </c>
       <c r="J22" t="s">
+        <v>4705</v>
+      </c>
+      <c r="K22" t="s">
+        <v>4457</v>
+      </c>
+      <c r="L22" t="s">
+        <v>4628</v>
+      </c>
+      <c r="M22" t="s">
+        <v>26</v>
+      </c>
+      <c r="N22" t="s">
+        <v>4630</v>
+      </c>
+      <c r="O22" t="s">
+        <v>4631</v>
+      </c>
+      <c r="P22" t="s">
+        <v>4628</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>4633</v>
+      </c>
+      <c r="R22" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" t="s">
+        <v>4687</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4687</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4682</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4686</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4440</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2697</v>
+      </c>
+      <c r="G23" t="s">
+        <v>4680</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4444</v>
+      </c>
+      <c r="I23" t="s">
+        <v>2696</v>
+      </c>
+      <c r="J23" t="s">
         <v>4683</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K23" t="s">
         <v>4684</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L23" t="s">
         <v>4681</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M23" t="s">
         <v>4633</v>
       </c>
-      <c r="N22" s="10" t="s">
+      <c r="N23" s="10" t="s">
         <v>4685</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N10" r:id="rId1" display="https://www.lcsc.com/product-detail/Light-Emitting-Diodes-LED_Worldsemi-WS2812B-Mini_C527089.html" xr:uid="{7B3563B0-676F-492C-A346-E0B4B21DFE92}"/>
-    <hyperlink ref="P16" r:id="rId2" display="https://www.lcsc.com/product-detail/MOSFETs_FUXINSEMI-SI2302_C6807797.html" xr:uid="{88ED9DD7-51B2-4FF9-80DF-03856639A5E8}"/>
+    <hyperlink ref="N11" r:id="rId1" display="https://www.lcsc.com/product-detail/Light-Emitting-Diodes-LED_Worldsemi-WS2812B-Mini_C527089.html" xr:uid="{7B3563B0-676F-492C-A346-E0B4B21DFE92}"/>
+    <hyperlink ref="P17" r:id="rId2" display="https://www.lcsc.com/product-detail/MOSFETs_FUXINSEMI-SI2302_C6807797.html" xr:uid="{88ED9DD7-51B2-4FF9-80DF-03856639A5E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -70278,7 +70344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05348336-C131-49E6-98A6-4A6B8B6DDA7F}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Moved LCSC Links for Misc Table
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Temp\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3452D018-D06D-4094-A20C-66369F3A8F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D388B8-445E-4955-A071-522017124BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" firstSheet="1" activeTab="2" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="1" activeTab="10" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16742" uniqueCount="4800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16746" uniqueCount="4800">
   <si>
     <t>Part Number</t>
   </si>
@@ -15155,10 +15155,10 @@
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="S1" sqref="S1:V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16394,10 +16394,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CA65D6-1BE4-4CF1-A255-E1F9C8CC291A}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16422,7 +16422,7 @@
     <col min="18" max="18" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16477,8 +16477,20 @@
       <c r="R1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" s="1" t="s">
+        <v>4658</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>4659</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>4660</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>4661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4356</v>
       </c>
@@ -16504,7 +16516,7 @@
         <v>4356</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4372</v>
       </c>
@@ -16530,7 +16542,7 @@
         <v>4372</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4377</v>
       </c>
@@ -16556,7 +16568,7 @@
         <v>4377</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4380</v>
       </c>
@@ -16582,7 +16594,7 @@
         <v>4380</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4381</v>
       </c>
@@ -16608,7 +16620,7 @@
         <v>4381</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4382</v>
       </c>
@@ -16634,7 +16646,7 @@
         <v>4382</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4383</v>
       </c>
@@ -16660,7 +16672,7 @@
         <v>4383</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4367</v>
       </c>
@@ -16686,7 +16698,7 @@
         <v>4367</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4366</v>
       </c>
@@ -16712,7 +16724,7 @@
         <v>4366</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4672</v>
       </c>
@@ -16737,18 +16749,6 @@
       <c r="I11" t="s">
         <v>4365</v>
       </c>
-      <c r="K11" t="s">
-        <v>4392</v>
-      </c>
-      <c r="L11" t="s">
-        <v>4393</v>
-      </c>
-      <c r="M11" t="s">
-        <v>4617</v>
-      </c>
-      <c r="N11" t="s">
-        <v>4394</v>
-      </c>
       <c r="O11" t="s">
         <v>4395</v>
       </c>
@@ -16761,8 +16761,20 @@
       <c r="R11" s="7" t="s">
         <v>4397</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11" t="s">
+        <v>4392</v>
+      </c>
+      <c r="T11" t="s">
+        <v>4393</v>
+      </c>
+      <c r="U11" t="s">
+        <v>4617</v>
+      </c>
+      <c r="V11" t="s">
+        <v>4394</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4407</v>
       </c>
@@ -16939,8 +16951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE72BB5-555B-4C95-9DE0-D4036F268B3F}">
   <dimension ref="A1:X345"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P315" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C315" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="S345" sqref="S345"/>

</xml_diff>

<commit_message>
LCSC part numbers added for resistors used in nightcones project
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C486B2-656F-4F27-BC91-6F8CD5F9F89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22325682-8430-4795-A7D9-1DF7502B67A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" firstSheet="1" activeTab="2" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16817" uniqueCount="4806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16832" uniqueCount="4812">
   <si>
     <t>Part Number</t>
   </si>
@@ -14464,6 +14464,24 @@
   </si>
   <si>
     <t>C21189</t>
+  </si>
+  <si>
+    <t>0603WAF1001T5E</t>
+  </si>
+  <si>
+    <t>C21190</t>
+  </si>
+  <si>
+    <t>0603WAF1002T5E</t>
+  </si>
+  <si>
+    <t>C25804</t>
+  </si>
+  <si>
+    <t>0603WAF1004T5E</t>
+  </si>
+  <si>
+    <t>C22935</t>
   </si>
 </sst>
 </file>
@@ -17045,10 +17063,10 @@
   <dimension ref="A1:Y345"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U3" sqref="U3"/>
+      <selection pane="bottomRight" activeCell="U148" sqref="U148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -20974,7 +20992,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="15.75">
+    <row r="65" spans="1:25" ht="15.75">
       <c r="A65" s="1" t="s">
         <v>141</v>
       </c>
@@ -21037,7 +21055,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="15.75">
+    <row r="66" spans="1:25" ht="15.75">
       <c r="A66" s="1" t="s">
         <v>143</v>
       </c>
@@ -21100,7 +21118,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="15.75">
+    <row r="67" spans="1:25" ht="15.75">
       <c r="A67" s="1" t="s">
         <v>145</v>
       </c>
@@ -21163,7 +21181,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="15.75">
+    <row r="68" spans="1:25" ht="15.75">
       <c r="A68" s="1" t="s">
         <v>149</v>
       </c>
@@ -21226,7 +21244,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="15.75">
+    <row r="69" spans="1:25" ht="15.75">
       <c r="A69" s="1" t="s">
         <v>151</v>
       </c>
@@ -21289,7 +21307,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="15.75">
+    <row r="70" spans="1:25" ht="15.75">
       <c r="A70" s="1" t="s">
         <v>153</v>
       </c>
@@ -21352,7 +21370,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="15.75">
+    <row r="71" spans="1:25" ht="15.75">
       <c r="A71" s="1" t="s">
         <v>155</v>
       </c>
@@ -21415,7 +21433,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="15.75">
+    <row r="72" spans="1:25" ht="15.75">
       <c r="A72" s="1" t="s">
         <v>157</v>
       </c>
@@ -21478,7 +21496,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="15.75">
+    <row r="73" spans="1:25" ht="15.75">
       <c r="A73" s="1" t="s">
         <v>159</v>
       </c>
@@ -21541,7 +21559,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="15.75">
+    <row r="74" spans="1:25" ht="15.75">
       <c r="A74" s="1" t="s">
         <v>161</v>
       </c>
@@ -21604,7 +21622,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="15.75">
+    <row r="75" spans="1:25" ht="15.75">
       <c r="A75" s="1" t="s">
         <v>163</v>
       </c>
@@ -21666,8 +21684,23 @@
       <c r="T75" s="1" t="s">
         <v>1411</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" ht="15.75">
+      <c r="U75" t="s">
+        <v>4803</v>
+      </c>
+      <c r="V75" t="s">
+        <v>4806</v>
+      </c>
+      <c r="W75" s="12" t="s">
+        <v>4617</v>
+      </c>
+      <c r="X75" t="s">
+        <v>4807</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" ht="15.75">
       <c r="A76" s="1" t="s">
         <v>165</v>
       </c>
@@ -21730,7 +21763,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="15.75">
+    <row r="77" spans="1:25" ht="15.75">
       <c r="A77" s="1" t="s">
         <v>167</v>
       </c>
@@ -21793,7 +21826,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="15.75">
+    <row r="78" spans="1:25" ht="15.75">
       <c r="A78" s="1" t="s">
         <v>169</v>
       </c>
@@ -21856,7 +21889,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="15.75">
+    <row r="79" spans="1:25" ht="15.75">
       <c r="A79" s="1" t="s">
         <v>171</v>
       </c>
@@ -21919,7 +21952,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="15.75">
+    <row r="80" spans="1:25" ht="15.75">
       <c r="A80" s="1" t="s">
         <v>175</v>
       </c>
@@ -22990,7 +23023,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="15.75">
+    <row r="97" spans="1:25" ht="15.75">
       <c r="A97" s="1" t="s">
         <v>223</v>
       </c>
@@ -23053,7 +23086,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="15.75">
+    <row r="98" spans="1:25" ht="15.75">
       <c r="A98" s="1" t="s">
         <v>225</v>
       </c>
@@ -23116,7 +23149,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="15.75">
+    <row r="99" spans="1:25" ht="15.75">
       <c r="A99" s="1" t="s">
         <v>229</v>
       </c>
@@ -23178,8 +23211,23 @@
       <c r="T99" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="100" spans="1:20" ht="15.75">
+      <c r="U99" t="s">
+        <v>4803</v>
+      </c>
+      <c r="V99" t="s">
+        <v>4808</v>
+      </c>
+      <c r="W99" s="12" t="s">
+        <v>4617</v>
+      </c>
+      <c r="X99" t="s">
+        <v>4809</v>
+      </c>
+      <c r="Y99" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" ht="15.75">
       <c r="A100" s="1" t="s">
         <v>233</v>
       </c>
@@ -23242,7 +23290,7 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="15.75">
+    <row r="101" spans="1:25" ht="15.75">
       <c r="A101" s="1" t="s">
         <v>235</v>
       </c>
@@ -23305,7 +23353,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="15.75">
+    <row r="102" spans="1:25" ht="15.75">
       <c r="A102" s="1" t="s">
         <v>239</v>
       </c>
@@ -23368,7 +23416,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="15.75">
+    <row r="103" spans="1:25" ht="15.75">
       <c r="A103" s="1" t="s">
         <v>243</v>
       </c>
@@ -23431,7 +23479,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="15.75">
+    <row r="104" spans="1:25" ht="15.75">
       <c r="A104" s="1" t="s">
         <v>247</v>
       </c>
@@ -23494,7 +23542,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="15.75">
+    <row r="105" spans="1:25" ht="15.75">
       <c r="A105" s="1" t="s">
         <v>251</v>
       </c>
@@ -23557,7 +23605,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="15.75">
+    <row r="106" spans="1:25" ht="15.75">
       <c r="A106" s="1" t="s">
         <v>255</v>
       </c>
@@ -23620,7 +23668,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="15.75">
+    <row r="107" spans="1:25" ht="15.75">
       <c r="A107" s="1" t="s">
         <v>257</v>
       </c>
@@ -23683,7 +23731,7 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="15.75">
+    <row r="108" spans="1:25" ht="15.75">
       <c r="A108" s="1" t="s">
         <v>259</v>
       </c>
@@ -23746,7 +23794,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="15.75">
+    <row r="109" spans="1:25" ht="15.75">
       <c r="A109" s="1" t="s">
         <v>263</v>
       </c>
@@ -23809,7 +23857,7 @@
         <v>1549</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="15.75">
+    <row r="110" spans="1:25" ht="15.75">
       <c r="A110" s="1" t="s">
         <v>265</v>
       </c>
@@ -23872,7 +23920,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="15.75">
+    <row r="111" spans="1:25" ht="15.75">
       <c r="A111" s="1" t="s">
         <v>267</v>
       </c>
@@ -23935,7 +23983,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="15.75">
+    <row r="112" spans="1:25" ht="15.75">
       <c r="A112" s="1" t="s">
         <v>269</v>
       </c>
@@ -25998,7 +26046,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="15.75">
+    <row r="145" spans="1:25" ht="15.75">
       <c r="A145" s="1" t="s">
         <v>365</v>
       </c>
@@ -26061,7 +26109,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="15.75">
+    <row r="146" spans="1:25" ht="15.75">
       <c r="A146" s="1" t="s">
         <v>367</v>
       </c>
@@ -26116,7 +26164,7 @@
       <c r="S146" s="1"/>
       <c r="T146" s="1"/>
     </row>
-    <row r="147" spans="1:20" ht="15.75">
+    <row r="147" spans="1:25" ht="15.75">
       <c r="A147" s="1" t="s">
         <v>369</v>
       </c>
@@ -26178,8 +26226,23 @@
       <c r="T147" s="1" t="s">
         <v>1703</v>
       </c>
-    </row>
-    <row r="148" spans="1:20" ht="15.75">
+      <c r="U147" t="s">
+        <v>4803</v>
+      </c>
+      <c r="V147" t="s">
+        <v>4810</v>
+      </c>
+      <c r="W147" t="s">
+        <v>4811</v>
+      </c>
+      <c r="X147" t="s">
+        <v>4617</v>
+      </c>
+      <c r="Y147" t="s">
+        <v>4802</v>
+      </c>
+    </row>
+    <row r="148" spans="1:25" ht="15.75">
       <c r="A148" s="1" t="s">
         <v>371</v>
       </c>
@@ -26234,7 +26297,7 @@
       <c r="S148" s="1"/>
       <c r="T148" s="1"/>
     </row>
-    <row r="149" spans="1:20" ht="15.75">
+    <row r="149" spans="1:25" ht="15.75">
       <c r="A149" s="1" t="s">
         <v>373</v>
       </c>
@@ -26297,7 +26360,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="15.75">
+    <row r="150" spans="1:25" ht="15.75">
       <c r="A150" s="1" t="s">
         <v>375</v>
       </c>
@@ -26352,7 +26415,7 @@
       <c r="S150" s="1"/>
       <c r="T150" s="1"/>
     </row>
-    <row r="151" spans="1:20" ht="15.75">
+    <row r="151" spans="1:25" ht="15.75">
       <c r="A151" s="1" t="s">
         <v>377</v>
       </c>
@@ -26415,7 +26478,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="15.75">
+    <row r="152" spans="1:25" ht="15.75">
       <c r="A152" s="1" t="s">
         <v>379</v>
       </c>
@@ -26470,7 +26533,7 @@
       <c r="S152" s="1"/>
       <c r="T152" s="1"/>
     </row>
-    <row r="153" spans="1:20" ht="15.75">
+    <row r="153" spans="1:25" ht="15.75">
       <c r="A153" s="1" t="s">
         <v>381</v>
       </c>
@@ -26525,7 +26588,7 @@
       <c r="S153" s="1"/>
       <c r="T153" s="1"/>
     </row>
-    <row r="154" spans="1:20" ht="15.75">
+    <row r="154" spans="1:25" ht="15.75">
       <c r="A154" s="1" t="s">
         <v>383</v>
       </c>
@@ -26588,7 +26651,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="15.75">
+    <row r="155" spans="1:25" ht="15.75">
       <c r="A155" s="1" t="s">
         <v>385</v>
       </c>
@@ -26651,7 +26714,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="15.75">
+    <row r="156" spans="1:25" ht="15.75">
       <c r="A156" s="1" t="s">
         <v>387</v>
       </c>
@@ -26706,7 +26769,7 @@
       <c r="S156" s="1"/>
       <c r="T156" s="1"/>
     </row>
-    <row r="157" spans="1:20" ht="15.75">
+    <row r="157" spans="1:25" ht="15.75">
       <c r="A157" s="1" t="s">
         <v>389</v>
       </c>
@@ -26761,7 +26824,7 @@
       <c r="S157" s="1"/>
       <c r="T157" s="1"/>
     </row>
-    <row r="158" spans="1:20" ht="15.75">
+    <row r="158" spans="1:25" ht="15.75">
       <c r="A158" s="1" t="s">
         <v>391</v>
       </c>
@@ -26816,7 +26879,7 @@
       <c r="S158" s="1"/>
       <c r="T158" s="1"/>
     </row>
-    <row r="159" spans="1:20" ht="15.75">
+    <row r="159" spans="1:25" ht="15.75">
       <c r="A159" s="1" t="s">
         <v>393</v>
       </c>
@@ -26871,7 +26934,7 @@
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
     </row>
-    <row r="160" spans="1:20" ht="15.75">
+    <row r="160" spans="1:25" ht="15.75">
       <c r="A160" s="1" t="s">
         <v>395</v>
       </c>

</xml_diff>

<commit_message>
Correction of WS2813E rotation
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBCCF81-9A35-41A5-A331-F27E399268A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E328C65E-A561-4490-889C-4CFECB90ED39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="10" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17016" uniqueCount="4875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17016" uniqueCount="4876">
   <si>
     <t>Part Number</t>
   </si>
@@ -14671,6 +14671,9 @@
   </si>
   <si>
     <t>21700 Battery cell for FSCH nightcone project</t>
+  </si>
+  <si>
+    <t>LEDM5050X165-6-NE</t>
   </si>
 </sst>
 </file>
@@ -15385,11 +15388,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8992C59-F5E3-466D-8132-19915B114D9C}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -15653,7 +15656,7 @@
         <v>3911</v>
       </c>
       <c r="I5" t="s">
-        <v>4864</v>
+        <v>4875</v>
       </c>
       <c r="J5" t="s">
         <v>4664</v>
@@ -16746,7 +16749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CA65D6-1BE4-4CF1-A255-E1F9C8CC291A}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LCSC supplier link of 470P/0603/50V/C0G adjusted
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E328C65E-A561-4490-889C-4CFECB90ED39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655FA932-091F-4674-AB9D-E06BEB694BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="3" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17016" uniqueCount="4876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17016" uniqueCount="4877">
   <si>
     <t>Part Number</t>
   </si>
@@ -14586,12 +14586,6 @@
     <t>C194323</t>
   </si>
   <si>
-    <t>C126566</t>
-  </si>
-  <si>
-    <t>GCM1885C1H471JA16D</t>
-  </si>
-  <si>
     <t>0603WAF4701T5E</t>
   </si>
   <si>
@@ -14674,6 +14668,15 @@
   </si>
   <si>
     <t>LEDM5050X165-6-NE</t>
+  </si>
+  <si>
+    <t>Walsin Tech Corp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT18N471J500CT </t>
+  </si>
+  <si>
+    <t>c458969</t>
   </si>
 </sst>
 </file>
@@ -15388,7 +15391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8992C59-F5E3-466D-8132-19915B114D9C}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -15518,7 +15521,7 @@
         <v>4419</v>
       </c>
       <c r="I2" t="s">
-        <v>4863</v>
+        <v>4861</v>
       </c>
       <c r="J2" t="s">
         <v>4661</v>
@@ -15565,7 +15568,7 @@
         <v>4420</v>
       </c>
       <c r="I3" t="s">
-        <v>4851</v>
+        <v>4849</v>
       </c>
       <c r="J3" t="s">
         <v>4662</v>
@@ -15609,7 +15612,7 @@
         <v>4419</v>
       </c>
       <c r="I4" t="s">
-        <v>4850</v>
+        <v>4848</v>
       </c>
       <c r="J4" t="s">
         <v>4663</v>
@@ -15656,7 +15659,7 @@
         <v>3911</v>
       </c>
       <c r="I5" t="s">
-        <v>4875</v>
+        <v>4873</v>
       </c>
       <c r="J5" t="s">
         <v>4664</v>
@@ -15703,7 +15706,7 @@
         <v>3911</v>
       </c>
       <c r="I6" t="s">
-        <v>4864</v>
+        <v>4862</v>
       </c>
       <c r="J6" t="s">
         <v>4665</v>
@@ -15750,7 +15753,7 @@
         <v>3911</v>
       </c>
       <c r="I7" t="s">
-        <v>4864</v>
+        <v>4862</v>
       </c>
       <c r="J7" t="s">
         <v>4683</v>
@@ -15797,7 +15800,7 @@
         <v>3911</v>
       </c>
       <c r="I8" t="s">
-        <v>4864</v>
+        <v>4862</v>
       </c>
       <c r="J8" t="s">
         <v>4844</v>
@@ -15844,7 +15847,7 @@
         <v>3911</v>
       </c>
       <c r="I9" t="s">
-        <v>4852</v>
+        <v>4850</v>
       </c>
       <c r="J9" t="s">
         <v>4666</v>
@@ -15891,7 +15894,7 @@
         <v>3911</v>
       </c>
       <c r="I10" t="s">
-        <v>4853</v>
+        <v>4851</v>
       </c>
       <c r="J10" t="s">
         <v>4667</v>
@@ -15938,7 +15941,7 @@
         <v>3911</v>
       </c>
       <c r="I11" t="s">
-        <v>4853</v>
+        <v>4851</v>
       </c>
       <c r="J11" t="s">
         <v>4668</v>
@@ -15985,7 +15988,7 @@
         <v>3911</v>
       </c>
       <c r="I12" t="s">
-        <v>4854</v>
+        <v>4852</v>
       </c>
       <c r="J12" t="s">
         <v>4669</v>
@@ -16032,7 +16035,7 @@
         <v>4419</v>
       </c>
       <c r="I13" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J13" t="s">
         <v>4670</v>
@@ -16079,7 +16082,7 @@
         <v>4420</v>
       </c>
       <c r="I14" t="s">
-        <v>4856</v>
+        <v>4854</v>
       </c>
       <c r="J14" t="s">
         <v>4671</v>
@@ -16126,7 +16129,7 @@
         <v>4419</v>
       </c>
       <c r="I15" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J15" t="s">
         <v>4432</v>
@@ -16185,7 +16188,7 @@
         <v>4419</v>
       </c>
       <c r="I16" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J16" t="s">
         <v>4438</v>
@@ -16244,7 +16247,7 @@
         <v>4419</v>
       </c>
       <c r="I17" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J17" t="s">
         <v>4445</v>
@@ -16303,7 +16306,7 @@
         <v>4419</v>
       </c>
       <c r="I18" t="s">
-        <v>4855</v>
+        <v>4853</v>
       </c>
       <c r="J18" t="s">
         <v>4672</v>
@@ -16362,7 +16365,7 @@
         <v>4419</v>
       </c>
       <c r="I19" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J19" t="s">
         <v>4673</v>
@@ -16406,7 +16409,7 @@
         <v>4419</v>
       </c>
       <c r="I20" t="s">
-        <v>4862</v>
+        <v>4860</v>
       </c>
       <c r="J20" t="s">
         <v>4567</v>
@@ -16465,7 +16468,7 @@
         <v>4419</v>
       </c>
       <c r="I21" t="s">
-        <v>4861</v>
+        <v>4859</v>
       </c>
       <c r="J21" t="s">
         <v>4674</v>
@@ -16512,7 +16515,7 @@
         <v>4419</v>
       </c>
       <c r="I22" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J22" t="s">
         <v>4675</v>
@@ -16559,7 +16562,7 @@
         <v>4419</v>
       </c>
       <c r="I23" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J23" t="s">
         <v>4676</v>
@@ -16618,7 +16621,7 @@
         <v>4419</v>
       </c>
       <c r="I24" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J24" t="s">
         <v>4654</v>
@@ -16666,7 +16669,7 @@
         <v>4419</v>
       </c>
       <c r="I25" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J25" t="s">
         <v>4688</v>
@@ -16713,7 +16716,7 @@
         <v>4419</v>
       </c>
       <c r="I26" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="J26" t="s">
         <v>4761</v>
@@ -17135,13 +17138,13 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>4872</v>
+        <v>4870</v>
       </c>
       <c r="B12" t="s">
-        <v>4872</v>
+        <v>4870</v>
       </c>
       <c r="C12" t="s">
-        <v>4871</v>
+        <v>4869</v>
       </c>
       <c r="D12" t="s">
         <v>4351</v>
@@ -17156,18 +17159,18 @@
         <v>4402</v>
       </c>
       <c r="I12" t="s">
-        <v>4870</v>
+        <v>4868</v>
       </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>4873</v>
+        <v>4871</v>
       </c>
       <c r="B13" t="s">
-        <v>4873</v>
+        <v>4871</v>
       </c>
       <c r="C13" t="s">
-        <v>4874</v>
+        <v>4872</v>
       </c>
       <c r="D13" t="s">
         <v>4351</v>
@@ -17182,7 +17185,7 @@
         <v>4402</v>
       </c>
       <c r="I13" t="s">
-        <v>4869</v>
+        <v>4867</v>
       </c>
     </row>
   </sheetData>
@@ -23075,13 +23078,13 @@
         <v>4786</v>
       </c>
       <c r="V91" t="s">
-        <v>4848</v>
+        <v>4846</v>
       </c>
       <c r="W91" s="1" t="s">
         <v>4604</v>
       </c>
       <c r="X91" t="s">
-        <v>4849</v>
+        <v>4847</v>
       </c>
       <c r="Y91" s="1" t="s">
         <v>4785</v>
@@ -38361,11 +38364,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8A1AAB-C407-4ADB-8694-9A4B002D9EDF}">
   <dimension ref="A1:Y97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="R13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W35" sqref="W35"/>
+      <selection pane="bottomRight" activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -40580,16 +40583,16 @@
         <v>710</v>
       </c>
       <c r="U34" s="12" t="s">
-        <v>4830</v>
+        <v>4874</v>
       </c>
       <c r="V34" t="s">
-        <v>4847</v>
+        <v>4875</v>
       </c>
       <c r="W34" t="s">
         <v>4604</v>
       </c>
       <c r="X34" s="12" t="s">
-        <v>4846</v>
+        <v>4876</v>
       </c>
       <c r="Y34" t="s">
         <v>4784</v>
@@ -72541,7 +72544,7 @@
         <v>4420</v>
       </c>
       <c r="J2" t="s">
-        <v>4859</v>
+        <v>4857</v>
       </c>
       <c r="U2" t="s">
         <v>4479</v>
@@ -72586,7 +72589,7 @@
         <v>4419</v>
       </c>
       <c r="J3" t="s">
-        <v>4857</v>
+        <v>4855</v>
       </c>
       <c r="U3" t="s">
         <v>4446</v>
@@ -72631,7 +72634,7 @@
         <v>4420</v>
       </c>
       <c r="J4" t="s">
-        <v>4858</v>
+        <v>4856</v>
       </c>
       <c r="U4" t="s">
         <v>4492</v>
@@ -72793,13 +72796,13 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>4865</v>
+        <v>4863</v>
       </c>
       <c r="B3" t="s">
-        <v>4865</v>
+        <v>4863</v>
       </c>
       <c r="C3" t="s">
-        <v>4866</v>
+        <v>4864</v>
       </c>
       <c r="D3" t="s">
         <v>4394</v>
@@ -72811,25 +72814,25 @@
         <v>4396</v>
       </c>
       <c r="H3" t="s">
-        <v>4865</v>
+        <v>4863</v>
       </c>
       <c r="I3" t="s">
         <v>4476</v>
       </c>
       <c r="J3" t="s">
-        <v>4865</v>
+        <v>4863</v>
       </c>
       <c r="U3" t="s">
         <v>4399</v>
       </c>
       <c r="V3" t="s">
-        <v>4867</v>
+        <v>4865</v>
       </c>
       <c r="W3" t="s">
         <v>4604</v>
       </c>
       <c r="X3" t="s">
-        <v>4868</v>
+        <v>4866</v>
       </c>
       <c r="Y3" t="s">
         <v>4784</v>

</xml_diff>

<commit_message>
I2C EEPROM ZD24C02B added
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D79B01-7ED6-4C7B-B52E-654DD0087E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CCD1D7-94F7-4F7F-9670-B3510AF7E42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="10" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22282" uniqueCount="6701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22297" uniqueCount="6707">
   <si>
     <t>Part Number</t>
   </si>
@@ -20149,6 +20149,24 @@
   </si>
   <si>
     <t>TC2070-NL</t>
+  </si>
+  <si>
+    <t>ZD24C02B</t>
+  </si>
+  <si>
+    <t>I2C-Compatible (2-wire) Serial EEPROM 2K bits</t>
+  </si>
+  <si>
+    <t>EEPROM_I2C_WP_3ADDR</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2402020955_Zetta-ZD24C02B-SSGMB_C5374786.pdf</t>
+  </si>
+  <si>
+    <t>ZD24C02B-SSGMB</t>
+  </si>
+  <si>
+    <t>C5374786</t>
   </si>
 </sst>
 </file>
@@ -20942,13 +20960,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8992C59-F5E3-466D-8132-19915B114D9C}">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I34" sqref="I34"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -22599,7 +22617,7 @@
         <v>6365</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:23">
       <c r="A33" t="s">
         <v>6420</v>
       </c>
@@ -22655,7 +22673,7 @@
         <v>6416</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:23">
       <c r="A34" t="s">
         <v>6425</v>
       </c>
@@ -22711,7 +22729,7 @@
         <v>6429</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:23">
       <c r="A35" t="s">
         <v>6434</v>
       </c>
@@ -22765,6 +22783,53 @@
       </c>
       <c r="V35" s="5" t="s">
         <v>6440</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
+      <c r="A36" t="s">
+        <v>6701</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6701</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6702</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4568</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6328</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2693</v>
+      </c>
+      <c r="G36" t="s">
+        <v>6703</v>
+      </c>
+      <c r="H36" t="s">
+        <v>4417</v>
+      </c>
+      <c r="I36" t="s">
+        <v>4849</v>
+      </c>
+      <c r="J36" t="s">
+        <v>6704</v>
+      </c>
+      <c r="S36" t="s">
+        <v>4568</v>
+      </c>
+      <c r="T36" t="s">
+        <v>6705</v>
+      </c>
+      <c r="U36" t="s">
+        <v>4601</v>
+      </c>
+      <c r="V36" t="s">
+        <v>6706</v>
+      </c>
+      <c r="W36" t="s">
+        <v>4780</v>
       </c>
     </row>
   </sheetData>
@@ -22782,8 +22847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CA65D6-1BE4-4CF1-A255-E1F9C8CC291A}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Type in Tag-Connect footprint corrected
</commit_message>
<xml_diff>
--- a/daniw_altium_lib.xlsx
+++ b/daniw_altium_lib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\ele\daniw_altium_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CCD1D7-94F7-4F7F-9670-B3510AF7E42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0629A6E9-DE63-4719-AD7D-D75A80BF6831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="9" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" firstSheet="1" activeTab="10" xr2:uid="{3DF4F140-3850-4A89-8CCA-7C160BF9B667}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -20079,9 +20079,6 @@
     <t>CON6</t>
   </si>
   <si>
-    <t>PCB/TAG-CONECT.PcbLib</t>
-  </si>
-  <si>
     <t>TC2030</t>
   </si>
   <si>
@@ -20167,6 +20164,9 @@
   </si>
   <si>
     <t>C5374786</t>
+  </si>
+  <si>
+    <t>PCB/TAG_CONNECT.PcbLib</t>
   </si>
 </sst>
 </file>
@@ -20962,7 +20962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8992C59-F5E3-466D-8132-19915B114D9C}">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -22787,13 +22787,13 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" t="s">
+        <v>6700</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6700</v>
+      </c>
+      <c r="C36" t="s">
         <v>6701</v>
-      </c>
-      <c r="B36" t="s">
-        <v>6701</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6702</v>
       </c>
       <c r="D36" t="s">
         <v>4568</v>
@@ -22805,7 +22805,7 @@
         <v>2693</v>
       </c>
       <c r="G36" t="s">
-        <v>6703</v>
+        <v>6702</v>
       </c>
       <c r="H36" t="s">
         <v>4417</v>
@@ -22814,19 +22814,19 @@
         <v>4849</v>
       </c>
       <c r="J36" t="s">
-        <v>6704</v>
+        <v>6703</v>
       </c>
       <c r="S36" t="s">
         <v>4568</v>
       </c>
       <c r="T36" t="s">
-        <v>6705</v>
+        <v>6704</v>
       </c>
       <c r="U36" t="s">
         <v>4601</v>
       </c>
       <c r="V36" t="s">
-        <v>6706</v>
+        <v>6705</v>
       </c>
       <c r="W36" t="s">
         <v>4780</v>
@@ -22847,8 +22847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CA65D6-1BE4-4CF1-A255-E1F9C8CC291A}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -23419,7 +23419,7 @@
         <v>6674</v>
       </c>
       <c r="C18" t="s">
-        <v>6693</v>
+        <v>6692</v>
       </c>
       <c r="D18" t="s">
         <v>6675</v>
@@ -23431,24 +23431,24 @@
         <v>6676</v>
       </c>
       <c r="H18" t="s">
+        <v>6706</v>
+      </c>
+      <c r="I18" t="s">
         <v>6677</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>6678</v>
-      </c>
-      <c r="J18" t="s">
-        <v>6679</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>6680</v>
+        <v>6679</v>
       </c>
       <c r="B19" t="s">
-        <v>6680</v>
+        <v>6679</v>
       </c>
       <c r="C19" t="s">
-        <v>6694</v>
+        <v>6693</v>
       </c>
       <c r="D19" t="s">
         <v>6675</v>
@@ -23460,24 +23460,24 @@
         <v>6676</v>
       </c>
       <c r="H19" t="s">
-        <v>6677</v>
+        <v>6706</v>
       </c>
       <c r="I19" t="s">
+        <v>6680</v>
+      </c>
+      <c r="J19" t="s">
         <v>6681</v>
-      </c>
-      <c r="J19" t="s">
-        <v>6682</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>6683</v>
+        <v>6682</v>
       </c>
       <c r="B20" t="s">
-        <v>6683</v>
+        <v>6682</v>
       </c>
       <c r="C20" t="s">
-        <v>6695</v>
+        <v>6694</v>
       </c>
       <c r="D20" t="s">
         <v>6675</v>
@@ -23486,27 +23486,27 @@
         <v>4472</v>
       </c>
       <c r="G20" t="s">
-        <v>6684</v>
+        <v>6683</v>
       </c>
       <c r="H20" t="s">
-        <v>6677</v>
+        <v>6706</v>
       </c>
       <c r="I20" t="s">
-        <v>6691</v>
+        <v>6690</v>
       </c>
       <c r="J20" t="s">
-        <v>6689</v>
+        <v>6688</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>6685</v>
+        <v>6684</v>
       </c>
       <c r="B21" t="s">
-        <v>6685</v>
+        <v>6684</v>
       </c>
       <c r="C21" t="s">
-        <v>6696</v>
+        <v>6695</v>
       </c>
       <c r="D21" t="s">
         <v>6675</v>
@@ -23515,24 +23515,24 @@
         <v>4472</v>
       </c>
       <c r="G21" t="s">
-        <v>6684</v>
+        <v>6683</v>
       </c>
       <c r="H21" t="s">
-        <v>6677</v>
+        <v>6706</v>
       </c>
       <c r="I21" t="s">
-        <v>6692</v>
+        <v>6691</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>6686</v>
+        <v>6685</v>
       </c>
       <c r="B22" t="s">
-        <v>6686</v>
+        <v>6685</v>
       </c>
       <c r="C22" t="s">
-        <v>6697</v>
+        <v>6696</v>
       </c>
       <c r="D22" t="s">
         <v>6675</v>
@@ -23541,27 +23541,27 @@
         <v>4472</v>
       </c>
       <c r="G22" t="s">
-        <v>6687</v>
+        <v>6686</v>
       </c>
       <c r="H22" t="s">
-        <v>6677</v>
+        <v>6706</v>
       </c>
       <c r="I22" t="s">
-        <v>6699</v>
+        <v>6698</v>
       </c>
       <c r="J22" t="s">
-        <v>6690</v>
+        <v>6689</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>6688</v>
+        <v>6687</v>
       </c>
       <c r="B23" t="s">
-        <v>6688</v>
+        <v>6687</v>
       </c>
       <c r="C23" t="s">
-        <v>6698</v>
+        <v>6697</v>
       </c>
       <c r="D23" t="s">
         <v>6675</v>
@@ -23570,13 +23570,13 @@
         <v>4472</v>
       </c>
       <c r="G23" t="s">
-        <v>6687</v>
+        <v>6686</v>
       </c>
       <c r="H23" t="s">
-        <v>6677</v>
+        <v>6706</v>
       </c>
       <c r="I23" t="s">
-        <v>6700</v>
+        <v>6699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>